<commit_message>
Add second floor map
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BG" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="122">
   <si>
     <t>y/x</t>
   </si>
@@ -196,12 +196,6 @@
     <t>Trap2</t>
   </si>
   <si>
-    <t>BUS1</t>
-  </si>
-  <si>
-    <t>BUS2</t>
-  </si>
-  <si>
     <t>Alpha1</t>
   </si>
   <si>
@@ -332,12 +326,75 @@
   </si>
   <si>
     <t>SSD6</t>
+  </si>
+  <si>
+    <t>0710</t>
+  </si>
+  <si>
+    <t>0709</t>
+  </si>
+  <si>
+    <t>0708</t>
+  </si>
+  <si>
+    <t>0707</t>
+  </si>
+  <si>
+    <t>0706</t>
+  </si>
+  <si>
+    <t>0705</t>
+  </si>
+  <si>
+    <t>0704</t>
+  </si>
+  <si>
+    <t>0610</t>
+  </si>
+  <si>
+    <t>0609</t>
+  </si>
+  <si>
+    <t>0608</t>
+  </si>
+  <si>
+    <t>0607</t>
+  </si>
+  <si>
+    <t>0606</t>
+  </si>
+  <si>
+    <t>0605</t>
+  </si>
+  <si>
+    <t>0604</t>
+  </si>
+  <si>
+    <t>0508</t>
+  </si>
+  <si>
+    <t>0507</t>
+  </si>
+  <si>
+    <t>0506</t>
+  </si>
+  <si>
+    <t>0505</t>
+  </si>
+  <si>
+    <t>0504</t>
+  </si>
+  <si>
+    <t>BTSO1</t>
+  </si>
+  <si>
+    <t>BTSO2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -668,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -903,38 +960,80 @@
     <xf numFmtId="1" fontId="1" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1242,7 +1341,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1252,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4:Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,20 +1365,20 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
+      <c r="Q1" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
       <c r="T1" s="57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F2" s="80" t="s">
+      <c r="F2" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="80"/>
+      <c r="G2" s="89"/>
       <c r="H2">
         <v>53</v>
       </c>
@@ -1374,7 +1473,7 @@
       </c>
       <c r="X4" s="6"/>
       <c r="Z4" s="60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AG4" s="6"/>
     </row>
@@ -1389,13 +1488,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="52" t="s">
         <v>97</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="52" t="s">
-        <v>99</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>8</v>
@@ -1415,15 +1514,15 @@
         <f>CONCATENATE(R15,N5,)</f>
         <v>0410</v>
       </c>
-      <c r="S5" s="86" t="str">
+      <c r="S5" s="84" t="str">
         <f>CONCATENATE(S15,N5,)</f>
         <v>0510</v>
       </c>
-      <c r="T5" s="87" t="str">
+      <c r="T5" s="85" t="str">
         <f>CONCATENATE(T15,N5)</f>
         <v>0610</v>
       </c>
-      <c r="U5" s="88" t="str">
+      <c r="U5" s="86" t="str">
         <f>CONCATENATE(U15,N5)</f>
         <v>0710</v>
       </c>
@@ -1434,7 +1533,7 @@
       </c>
       <c r="X5" s="6"/>
       <c r="Z5" s="59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AG5" s="6"/>
     </row>
@@ -1451,13 +1550,13 @@
         <v>9</v>
       </c>
       <c r="F6" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="53" t="s">
         <v>100</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>102</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>8</v>
@@ -1468,7 +1567,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="N6" s="54" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="14"/>
@@ -1480,7 +1579,7 @@
         <f>CONCATENATE(R15,N6,)</f>
         <v>0409</v>
       </c>
-      <c r="S6" s="89" t="str">
+      <c r="S6" s="87" t="str">
         <f>CONCATENATE(S15,N6,)</f>
         <v>0509</v>
       </c>
@@ -1488,7 +1587,7 @@
         <f>CONCATENATE(T15,N6)</f>
         <v>0609</v>
       </c>
-      <c r="U6" s="90" t="str">
+      <c r="U6" s="88" t="str">
         <f>CONCATENATE(U15,N6)</f>
         <v>0709</v>
       </c>
@@ -1499,7 +1598,7 @@
       </c>
       <c r="X6" s="6"/>
       <c r="Z6" s="61" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AG6" s="6"/>
     </row>
@@ -1533,7 +1632,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="N7" s="54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="14"/>
@@ -1564,7 +1663,7 @@
       </c>
       <c r="X7" s="6"/>
       <c r="Z7" s="62" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AG7" s="6"/>
     </row>
@@ -1598,7 +1697,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="N8" s="54" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="14"/>
@@ -1664,7 +1763,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="N9" s="54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="14"/>
@@ -1684,7 +1783,7 @@
         <f>CONCATENATE(T15,N9)</f>
         <v>0606</v>
       </c>
-      <c r="U9" s="84" t="str">
+      <c r="U9" s="82" t="str">
         <f>CONCATENATE(U15,N9)</f>
         <v>0706</v>
       </c>
@@ -1727,7 +1826,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="N10" s="54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="14"/>
@@ -1739,11 +1838,11 @@
         <f>CONCATENATE(R15,N10,)</f>
         <v>0405</v>
       </c>
-      <c r="S10" s="82" t="str">
+      <c r="S10" s="80" t="str">
         <f>CONCATENATE(S15,N10)</f>
         <v>0505</v>
       </c>
-      <c r="T10" s="83" t="str">
+      <c r="T10" s="81" t="str">
         <f>CONCATENATE(T15,N10)</f>
         <v>0605</v>
       </c>
@@ -1788,7 +1887,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="N11" s="54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
@@ -1797,7 +1896,7 @@
         <f>CONCATENATE(R15,N11,)</f>
         <v>0404</v>
       </c>
-      <c r="S11" s="85" t="str">
+      <c r="S11" s="83" t="str">
         <f>CONCATENATE(S15,N11)</f>
         <v>0504</v>
       </c>
@@ -1846,7 +1945,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="N12" s="54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
@@ -1895,7 +1994,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="34"/>
       <c r="N13" s="54" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="6"/>
@@ -1925,7 +2024,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="34"/>
       <c r="N14" s="54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O14" s="29"/>
       <c r="P14" s="18"/>
@@ -1977,31 +2076,31 @@
         <v>0</v>
       </c>
       <c r="O15" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="P15" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q15" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="P15" s="54" t="s">
+      <c r="R15" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="Q15" s="54" t="s">
+      <c r="S15" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="R15" s="55" t="s">
+      <c r="T15" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="S15" s="56" t="s">
+      <c r="U15" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="T15" s="56" t="s">
+      <c r="V15" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="U15" s="56" t="s">
+      <c r="W15" s="55" t="s">
         <v>88</v>
-      </c>
-      <c r="V15" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="W15" s="55" t="s">
-        <v>90</v>
       </c>
       <c r="X15" s="54">
         <v>10</v>
@@ -2019,11 +2118,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="81" t="s">
+      <c r="B20" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2042,32 +2141,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K15"/>
+  <dimension ref="B1:W15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="10" width="7.140625" customWidth="1"/>
+    <col min="2" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="10" width="7.140625" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G2" s="80" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="G2" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="80"/>
+      <c r="H2" s="89"/>
       <c r="I2">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>12</v>
       </c>
@@ -2080,49 +2182,89 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="1">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>11</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <v>11</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>10</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="9" t="s">
-        <v>57</v>
+      <c r="H5" s="35" t="s">
+        <v>120</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <v>10</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="92"/>
+      <c r="S5" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="T5" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="U5" s="22"/>
+      <c r="W5" s="60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>9</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="6"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="29" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="14" t="s">
@@ -2130,15 +2272,33 @@
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>9</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="92"/>
+      <c r="S6" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="T6" s="96" t="s">
+        <v>102</v>
+      </c>
+      <c r="U6" s="22"/>
+      <c r="W6" s="59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="14"/>
+      <c r="F7" s="91"/>
       <c r="G7" s="17" t="s">
         <v>49</v>
       </c>
@@ -2150,15 +2310,35 @@
       </c>
       <c r="J7" s="22"/>
       <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <v>8</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="91"/>
+      <c r="R7" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="S7" s="98" t="s">
+        <v>110</v>
+      </c>
+      <c r="T7" s="96" t="s">
+        <v>103</v>
+      </c>
+      <c r="U7" s="22"/>
+      <c r="W7" s="61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="14"/>
+      <c r="F8" s="91"/>
       <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
@@ -2170,15 +2350,35 @@
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="22"/>
-    </row>
-    <row r="9" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <v>7</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="91"/>
+      <c r="R8" s="95" t="s">
+        <v>116</v>
+      </c>
+      <c r="S8" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="T8" s="99" t="s">
+        <v>104</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="W8" s="62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="14"/>
+      <c r="F9" s="91"/>
       <c r="G9" s="28" t="s">
         <v>51</v>
       </c>
@@ -2190,15 +2390,32 @@
       </c>
       <c r="J9" s="22"/>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <v>6</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="91"/>
+      <c r="R9" s="101" t="s">
+        <v>117</v>
+      </c>
+      <c r="S9" s="103" t="s">
+        <v>112</v>
+      </c>
+      <c r="T9" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="U9" s="22"/>
+    </row>
+    <row r="10" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="38" t="s">
         <v>52</v>
       </c>
@@ -2210,15 +2427,32 @@
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="100" t="s">
+        <v>118</v>
+      </c>
+      <c r="S10" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="T10" s="96" t="s">
+        <v>106</v>
+      </c>
+      <c r="U10" s="22"/>
+    </row>
+    <row r="11" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="6"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="39" t="s">
         <v>53</v>
       </c>
@@ -2230,22 +2464,50 @@
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <v>4</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="101" t="s">
+        <v>119</v>
+      </c>
+      <c r="S11" s="97" t="s">
+        <v>114</v>
+      </c>
+      <c r="T11" s="104" t="s">
+        <v>107</v>
+      </c>
+      <c r="U11" s="22"/>
+    </row>
+    <row r="12" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>3</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <v>3</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+    </row>
+    <row r="13" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -2258,8 +2520,19 @@
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34"/>
-    </row>
-    <row r="14" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="1">
+        <v>2</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+    </row>
+    <row r="14" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -2272,8 +2545,19 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="34"/>
-    </row>
-    <row r="15" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="29"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+    </row>
+    <row r="15" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2286,7 +2570,7 @@
       <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="1">
         <v>4</v>
       </c>
       <c r="G15" s="4">
@@ -2299,6 +2583,33 @@
         <v>7</v>
       </c>
       <c r="J15" s="4">
+        <v>8</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>4</v>
+      </c>
+      <c r="R15" s="4">
+        <v>5</v>
+      </c>
+      <c r="S15" s="4">
+        <v>6</v>
+      </c>
+      <c r="T15" s="4">
+        <v>7</v>
+      </c>
+      <c r="U15" s="4">
         <v>8</v>
       </c>
     </row>
@@ -2307,6 +2618,7 @@
     <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2329,10 +2641,10 @@
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="80"/>
+      <c r="F2" s="89"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -2373,10 +2685,10 @@
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
       <c r="H5" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J5" s="22"/>
     </row>
@@ -2393,7 +2705,7 @@
         <v>29</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J6" s="22"/>
     </row>
@@ -2431,7 +2743,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J8" s="5"/>
     </row>
@@ -2481,10 +2793,10 @@
       <c r="F11" s="1"/>
       <c r="G11" s="14"/>
       <c r="H11" s="29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J11" s="22"/>
     </row>
@@ -2583,10 +2895,10 @@
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="80"/>
+      <c r="F2" s="89"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -2627,10 +2939,10 @@
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
       <c r="H5" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -2644,10 +2956,10 @@
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
       <c r="H6" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -2660,13 +2972,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>71</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -2679,13 +2991,13 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>74</v>
       </c>
       <c r="J8" s="2"/>
     </row>
@@ -2698,13 +3010,13 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>77</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -2718,10 +3030,10 @@
       <c r="F10" s="1"/>
       <c r="G10" s="10"/>
       <c r="H10" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -2735,10 +3047,10 @@
       <c r="F11" s="1"/>
       <c r="G11" s="14"/>
       <c r="H11" s="29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J11" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add third floor map
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="BG" sheetId="1" r:id="rId1"/>
+    <sheet name="First floor" sheetId="1" r:id="rId1"/>
     <sheet name="Second floor" sheetId="2" r:id="rId2"/>
     <sheet name="Third floor" sheetId="3" r:id="rId3"/>
     <sheet name="Fourth floor" sheetId="4" r:id="rId4"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
   <si>
     <t>y/x</t>
   </si>
@@ -208,12 +208,6 @@
     <t>Trap3</t>
   </si>
   <si>
-    <t>MKBO1</t>
-  </si>
-  <si>
-    <t>MKBO2</t>
-  </si>
-  <si>
     <t>Leeg1</t>
   </si>
   <si>
@@ -389,6 +383,63 @@
   </si>
   <si>
     <t>BTSO2</t>
+  </si>
+  <si>
+    <t>061002</t>
+  </si>
+  <si>
+    <t>060902</t>
+  </si>
+  <si>
+    <t>060802</t>
+  </si>
+  <si>
+    <t>060702</t>
+  </si>
+  <si>
+    <t>060602</t>
+  </si>
+  <si>
+    <t>060502</t>
+  </si>
+  <si>
+    <t>060402</t>
+  </si>
+  <si>
+    <t>071002</t>
+  </si>
+  <si>
+    <t>070902</t>
+  </si>
+  <si>
+    <t>070802</t>
+  </si>
+  <si>
+    <t>070702</t>
+  </si>
+  <si>
+    <t>070602</t>
+  </si>
+  <si>
+    <t>070502</t>
+  </si>
+  <si>
+    <t>070402</t>
+  </si>
+  <si>
+    <t>050802</t>
+  </si>
+  <si>
+    <t>050702</t>
+  </si>
+  <si>
+    <t>050602</t>
+  </si>
+  <si>
+    <t>Arcturis</t>
+  </si>
+  <si>
+    <t>Castor</t>
   </si>
 </sst>
 </file>
@@ -725,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -987,52 +1038,85 @@
     <xf numFmtId="1" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1041,6 +1125,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1365,20 +1454,20 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="89" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
+      <c r="Q1" s="103" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
       <c r="T1" s="57" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="89"/>
+      <c r="G2" s="103"/>
       <c r="H2">
         <v>53</v>
       </c>
@@ -1473,7 +1562,7 @@
       </c>
       <c r="X4" s="6"/>
       <c r="Z4" s="60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AG4" s="6"/>
     </row>
@@ -1488,13 +1577,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="52" t="s">
         <v>95</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="H5" s="52" t="s">
-        <v>97</v>
       </c>
       <c r="I5" s="27" t="s">
         <v>8</v>
@@ -1533,7 +1622,7 @@
       </c>
       <c r="X5" s="6"/>
       <c r="Z5" s="59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AG5" s="6"/>
     </row>
@@ -1550,13 +1639,13 @@
         <v>9</v>
       </c>
       <c r="F6" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="53" t="s">
         <v>98</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>100</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>8</v>
@@ -1567,7 +1656,7 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="N6" s="54" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="14"/>
@@ -1598,7 +1687,7 @@
       </c>
       <c r="X6" s="6"/>
       <c r="Z6" s="61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AG6" s="6"/>
     </row>
@@ -1632,7 +1721,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="N7" s="54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="14"/>
@@ -1663,7 +1752,7 @@
       </c>
       <c r="X7" s="6"/>
       <c r="Z7" s="62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="AG7" s="6"/>
     </row>
@@ -1697,7 +1786,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="N8" s="54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="14"/>
@@ -1763,7 +1852,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="N9" s="54" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="14"/>
@@ -1826,7 +1915,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="N10" s="54" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="14"/>
@@ -1887,7 +1976,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="N11" s="54" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
@@ -1945,7 +2034,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="N12" s="54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
@@ -1994,7 +2083,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="34"/>
       <c r="N13" s="54" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="6"/>
@@ -2024,7 +2113,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="34"/>
       <c r="N14" s="54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O14" s="29"/>
       <c r="P14" s="18"/>
@@ -2076,31 +2165,31 @@
         <v>0</v>
       </c>
       <c r="O15" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="P15" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q15" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="P15" s="54" t="s">
+      <c r="R15" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="Q15" s="54" t="s">
+      <c r="S15" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="55" t="s">
+      <c r="T15" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="56" t="s">
+      <c r="U15" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="T15" s="56" t="s">
+      <c r="V15" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="U15" s="56" t="s">
+      <c r="W15" s="55" t="s">
         <v>86</v>
-      </c>
-      <c r="V15" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="W15" s="55" t="s">
-        <v>88</v>
       </c>
       <c r="X15" s="54">
         <v>10</v>
@@ -2118,11 +2207,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="90" t="s">
+      <c r="B20" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="90"/>
-      <c r="D20" s="90"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2143,8 +2232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5:W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,10 +2250,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="89"/>
+      <c r="H2" s="103"/>
       <c r="I2">
         <v>19</v>
       </c>
@@ -2229,10 +2318,10 @@
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
       <c r="H5" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="6"/>
@@ -2243,16 +2332,16 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="92"/>
-      <c r="S5" s="93" t="s">
-        <v>108</v>
-      </c>
-      <c r="T5" s="94" t="s">
-        <v>101</v>
+      <c r="R5" s="90"/>
+      <c r="S5" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="T5" s="92" t="s">
+        <v>99</v>
       </c>
       <c r="U5" s="22"/>
       <c r="W5" s="60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2279,16 +2368,16 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="92"/>
-      <c r="S6" s="97" t="s">
-        <v>109</v>
-      </c>
-      <c r="T6" s="96" t="s">
-        <v>102</v>
+      <c r="R6" s="90"/>
+      <c r="S6" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="T6" s="94" t="s">
+        <v>100</v>
       </c>
       <c r="U6" s="22"/>
       <c r="W6" s="59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,7 +2387,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="91"/>
+      <c r="F7" s="89"/>
       <c r="G7" s="17" t="s">
         <v>49</v>
       </c>
@@ -2316,19 +2405,19 @@
       <c r="N7" s="5"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="100" t="s">
-        <v>115</v>
-      </c>
-      <c r="S7" s="98" t="s">
-        <v>110</v>
-      </c>
-      <c r="T7" s="96" t="s">
-        <v>103</v>
+      <c r="Q7" s="89"/>
+      <c r="R7" s="98" t="s">
+        <v>113</v>
+      </c>
+      <c r="S7" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="T7" s="94" t="s">
+        <v>101</v>
       </c>
       <c r="U7" s="22"/>
       <c r="W7" s="61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2338,7 +2427,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="91"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
@@ -2356,19 +2445,19 @@
       <c r="N8" s="5"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="91"/>
-      <c r="R8" s="95" t="s">
-        <v>116</v>
-      </c>
-      <c r="S8" s="98" t="s">
-        <v>111</v>
-      </c>
-      <c r="T8" s="99" t="s">
-        <v>104</v>
+      <c r="Q8" s="89"/>
+      <c r="R8" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="S8" s="96" t="s">
+        <v>109</v>
+      </c>
+      <c r="T8" s="97" t="s">
+        <v>102</v>
       </c>
       <c r="U8" s="5"/>
       <c r="W8" s="62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2378,7 +2467,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="91"/>
+      <c r="F9" s="89"/>
       <c r="G9" s="28" t="s">
         <v>51</v>
       </c>
@@ -2396,15 +2485,15 @@
       <c r="N9" s="5"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="101" t="s">
-        <v>117</v>
-      </c>
-      <c r="S9" s="103" t="s">
-        <v>112</v>
-      </c>
-      <c r="T9" s="102" t="s">
-        <v>105</v>
+      <c r="Q9" s="89"/>
+      <c r="R9" s="99" t="s">
+        <v>115</v>
+      </c>
+      <c r="S9" s="101" t="s">
+        <v>110</v>
+      </c>
+      <c r="T9" s="100" t="s">
+        <v>103</v>
       </c>
       <c r="U9" s="22"/>
     </row>
@@ -2434,14 +2523,14 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="100" t="s">
-        <v>118</v>
-      </c>
-      <c r="S10" s="95" t="s">
-        <v>113</v>
-      </c>
-      <c r="T10" s="96" t="s">
-        <v>106</v>
+      <c r="R10" s="98" t="s">
+        <v>116</v>
+      </c>
+      <c r="S10" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="T10" s="94" t="s">
+        <v>104</v>
       </c>
       <c r="U10" s="22"/>
     </row>
@@ -2471,14 +2560,14 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="101" t="s">
-        <v>119</v>
-      </c>
-      <c r="S11" s="97" t="s">
-        <v>114</v>
-      </c>
-      <c r="T11" s="104" t="s">
-        <v>107</v>
+      <c r="R11" s="99" t="s">
+        <v>117</v>
+      </c>
+      <c r="S11" s="95" t="s">
+        <v>112</v>
+      </c>
+      <c r="T11" s="102" t="s">
+        <v>105</v>
       </c>
       <c r="U11" s="22"/>
     </row>
@@ -2624,32 +2713,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:W15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="10" width="7.140625" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E2" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="89"/>
+      <c r="F2" s="103"/>
       <c r="G2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>12</v>
       </c>
@@ -2661,8 +2751,19 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="1">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>11</v>
       </c>
@@ -2674,8 +2775,19 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <v>11</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>10</v>
       </c>
@@ -2691,8 +2803,26 @@
         <v>58</v>
       </c>
       <c r="J5" s="22"/>
-    </row>
-    <row r="6" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <v>10</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="91" t="s">
+        <v>120</v>
+      </c>
+      <c r="T5" s="92" t="s">
+        <v>127</v>
+      </c>
+      <c r="U5" s="22"/>
+      <c r="W5" s="60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>9</v>
       </c>
@@ -2701,15 +2831,33 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="29" t="s">
         <v>29</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>59</v>
       </c>
       <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>9</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="95" t="s">
+        <v>121</v>
+      </c>
+      <c r="T6" s="94" t="s">
+        <v>128</v>
+      </c>
+      <c r="U6" s="22"/>
+      <c r="W6" s="59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8</v>
       </c>
@@ -2727,8 +2875,28 @@
         <v>30</v>
       </c>
       <c r="J7" s="22"/>
-    </row>
-    <row r="8" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <v>8</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="S7" s="96" t="s">
+        <v>122</v>
+      </c>
+      <c r="T7" s="94" t="s">
+        <v>129</v>
+      </c>
+      <c r="U7" s="22"/>
+      <c r="W7" s="61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -2746,8 +2914,28 @@
         <v>60</v>
       </c>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <v>7</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="93" t="s">
+        <v>135</v>
+      </c>
+      <c r="S8" s="115" t="s">
+        <v>123</v>
+      </c>
+      <c r="T8" s="97" t="s">
+        <v>130</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="W8" s="62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -2765,8 +2953,25 @@
         <v>36</v>
       </c>
       <c r="J9" s="22"/>
-    </row>
-    <row r="10" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <v>6</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="99" t="s">
+        <v>136</v>
+      </c>
+      <c r="S9" s="101" t="s">
+        <v>124</v>
+      </c>
+      <c r="T9" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="U9" s="22"/>
+    </row>
+    <row r="10" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -2778,12 +2983,27 @@
       <c r="H10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="33" t="s">
         <v>34</v>
       </c>
       <c r="J10" s="22"/>
-    </row>
-    <row r="11" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="113"/>
+      <c r="S10" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="T10" s="102" t="s">
+        <v>132</v>
+      </c>
+      <c r="U10" s="22"/>
+    </row>
+    <row r="11" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -2793,14 +3013,29 @@
       <c r="F11" s="1"/>
       <c r="G11" s="14"/>
       <c r="H11" s="29" t="s">
-        <v>61</v>
+        <v>138</v>
       </c>
       <c r="I11" s="33" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="J11" s="22"/>
-    </row>
-    <row r="12" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <v>4</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="114"/>
+      <c r="S11" s="95" t="s">
+        <v>126</v>
+      </c>
+      <c r="T11" s="102" t="s">
+        <v>133</v>
+      </c>
+      <c r="U11" s="22"/>
+    </row>
+    <row r="12" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -2812,8 +3047,19 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <v>3</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+    </row>
+    <row r="13" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -2825,8 +3071,19 @@
       <c r="H13" s="34"/>
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="1">
+        <v>2</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+    </row>
+    <row r="14" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -2838,8 +3095,19 @@
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="29"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+    </row>
+    <row r="15" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2865,6 +3133,33 @@
         <v>7</v>
       </c>
       <c r="J15" s="4">
+        <v>8</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>4</v>
+      </c>
+      <c r="R15" s="4">
+        <v>5</v>
+      </c>
+      <c r="S15" s="4">
+        <v>6</v>
+      </c>
+      <c r="T15" s="4">
+        <v>7</v>
+      </c>
+      <c r="U15" s="4">
         <v>8</v>
       </c>
     </row>
@@ -2873,37 +3168,39 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:W15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="10" width="7.140625" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E2" s="89" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E2" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="89"/>
+      <c r="F2" s="103"/>
       <c r="G2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>12</v>
       </c>
@@ -2915,8 +3212,19 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="1">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>11</v>
       </c>
@@ -2928,8 +3236,19 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <v>11</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>10</v>
       </c>
@@ -2939,14 +3258,32 @@
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
       <c r="H5" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <v>10</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="105" t="s">
+        <v>61</v>
+      </c>
+      <c r="T5" s="106" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" s="1"/>
+      <c r="W5" s="60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>9</v>
       </c>
@@ -2956,14 +3293,32 @@
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
       <c r="H6" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <v>9</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="107" t="s">
+        <v>63</v>
+      </c>
+      <c r="T6" s="108" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="1"/>
+      <c r="W6" s="59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8</v>
       </c>
@@ -2972,17 +3327,37 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>69</v>
-      </c>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <v>8</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="105" t="s">
+        <v>65</v>
+      </c>
+      <c r="S7" s="109" t="s">
+        <v>66</v>
+      </c>
+      <c r="T7" s="108" t="s">
+        <v>67</v>
+      </c>
+      <c r="U7" s="1"/>
+      <c r="W7" s="61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -2991,17 +3366,37 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>72</v>
-      </c>
       <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <v>7</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="107" t="s">
+        <v>68</v>
+      </c>
+      <c r="S8" s="109" t="s">
+        <v>69</v>
+      </c>
+      <c r="T8" s="110" t="s">
+        <v>70</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="W8" s="62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3010,17 +3405,34 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>75</v>
-      </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <v>6</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="111" t="s">
+        <v>71</v>
+      </c>
+      <c r="S9" s="110" t="s">
+        <v>72</v>
+      </c>
+      <c r="T9" s="108" t="s">
+        <v>73</v>
+      </c>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -3030,14 +3442,29 @@
       <c r="F10" s="1"/>
       <c r="G10" s="10"/>
       <c r="H10" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I10" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T10" s="108" t="s">
+        <v>74</v>
+      </c>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -3047,14 +3474,29 @@
       <c r="F11" s="1"/>
       <c r="G11" s="14"/>
       <c r="H11" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I11" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="M11" s="1">
+        <v>4</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="111" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T11" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3066,8 +3508,19 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <v>3</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -3076,8 +3529,16 @@
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
-    </row>
-    <row r="14" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="1">
+        <v>2</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+    </row>
+    <row r="14" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -3089,8 +3550,19 @@
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="2:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="29"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="18"/>
+    </row>
+    <row r="15" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -3116,6 +3588,33 @@
         <v>7</v>
       </c>
       <c r="J15" s="4">
+        <v>8</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>4</v>
+      </c>
+      <c r="R15" s="4">
+        <v>5</v>
+      </c>
+      <c r="S15" s="4">
+        <v>6</v>
+      </c>
+      <c r="T15" s="4">
+        <v>7</v>
+      </c>
+      <c r="U15" s="4">
         <v>8</v>
       </c>
     </row>
@@ -3124,5 +3623,6 @@
     <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add fourth floor map
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="First floor" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1080,43 +1080,22 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1454,20 +1433,20 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="103" t="s">
+      <c r="Q1" s="106" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="103"/>
-      <c r="S1" s="103"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
       <c r="T1" s="57" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F2" s="103" t="s">
+      <c r="F2" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="103"/>
+      <c r="G2" s="106"/>
       <c r="H2">
         <v>53</v>
       </c>
@@ -2207,11 +2186,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2250,10 +2229,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="G2" s="103" t="s">
+      <c r="G2" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="103"/>
+      <c r="H2" s="106"/>
       <c r="I2">
         <v>19</v>
       </c>
@@ -2715,7 +2694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -2731,10 +2710,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="103"/>
+      <c r="F2" s="106"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -2924,7 +2903,7 @@
       <c r="R8" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="S8" s="115" t="s">
+      <c r="S8" s="105" t="s">
         <v>123</v>
       </c>
       <c r="T8" s="97" t="s">
@@ -2994,7 +2973,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="113"/>
+      <c r="R10" s="103"/>
       <c r="S10" s="93" t="s">
         <v>125</v>
       </c>
@@ -3026,7 +3005,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="114"/>
+      <c r="R11" s="104"/>
       <c r="S11" s="95" t="s">
         <v>126</v>
       </c>
@@ -3176,8 +3155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" activeCellId="1" sqref="S5:T11 R7:R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,10 +3171,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="103"/>
+      <c r="F2" s="106"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -3271,12 +3250,12 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="105" t="s">
-        <v>61</v>
-      </c>
-      <c r="T5" s="106" t="s">
-        <v>62</v>
+      <c r="R5" s="90"/>
+      <c r="S5" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="T5" s="92" t="s">
+        <v>99</v>
       </c>
       <c r="U5" s="1"/>
       <c r="W5" s="60" t="s">
@@ -3306,12 +3285,12 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="107" t="s">
-        <v>63</v>
-      </c>
-      <c r="T6" s="108" t="s">
-        <v>64</v>
+      <c r="R6" s="90"/>
+      <c r="S6" s="93" t="s">
+        <v>107</v>
+      </c>
+      <c r="T6" s="94" t="s">
+        <v>100</v>
       </c>
       <c r="U6" s="1"/>
       <c r="W6" s="59" t="s">
@@ -3343,14 +3322,14 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="105" t="s">
-        <v>65</v>
-      </c>
-      <c r="S7" s="109" t="s">
-        <v>66</v>
-      </c>
-      <c r="T7" s="108" t="s">
-        <v>67</v>
+      <c r="R7" s="91" t="s">
+        <v>113</v>
+      </c>
+      <c r="S7" s="96" t="s">
+        <v>108</v>
+      </c>
+      <c r="T7" s="94" t="s">
+        <v>101</v>
       </c>
       <c r="U7" s="1"/>
       <c r="W7" s="61" t="s">
@@ -3382,14 +3361,14 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="107" t="s">
-        <v>68</v>
-      </c>
-      <c r="S8" s="109" t="s">
-        <v>69</v>
-      </c>
-      <c r="T8" s="110" t="s">
-        <v>70</v>
+      <c r="R8" s="93" t="s">
+        <v>114</v>
+      </c>
+      <c r="S8" s="96" t="s">
+        <v>109</v>
+      </c>
+      <c r="T8" s="108" t="s">
+        <v>102</v>
       </c>
       <c r="U8" s="2"/>
       <c r="W8" s="62" t="s">
@@ -3421,14 +3400,14 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="111" t="s">
-        <v>71</v>
-      </c>
-      <c r="S9" s="110" t="s">
-        <v>72</v>
-      </c>
-      <c r="T9" s="108" t="s">
-        <v>73</v>
+      <c r="R9" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="S9" s="108" t="s">
+        <v>110</v>
+      </c>
+      <c r="T9" s="94" t="s">
+        <v>103</v>
       </c>
       <c r="U9" s="1"/>
     </row>
@@ -3455,12 +3434,12 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="107" t="s">
-        <v>76</v>
-      </c>
-      <c r="T10" s="108" t="s">
-        <v>74</v>
+      <c r="R10" s="103"/>
+      <c r="S10" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="T10" s="94" t="s">
+        <v>104</v>
       </c>
       <c r="U10" s="1"/>
     </row>
@@ -3487,12 +3466,12 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="111" t="s">
-        <v>77</v>
-      </c>
-      <c r="T11" s="112" t="s">
-        <v>75</v>
+      <c r="R11" s="104"/>
+      <c r="S11" s="95" t="s">
+        <v>112</v>
+      </c>
+      <c r="T11" s="102" t="s">
+        <v>105</v>
       </c>
       <c r="U11" s="1"/>
     </row>

</xml_diff>

<commit_message>
Add code to lock doors on room 060600
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="First floor" sheetId="1" r:id="rId1"/>
@@ -1089,14 +1089,14 @@
     <xf numFmtId="49" fontId="1" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1419,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Z4" sqref="Z4:Z7"/>
     </sheetView>
   </sheetViews>
@@ -1433,20 +1433,20 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="106" t="s">
+      <c r="Q1" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="106"/>
-      <c r="S1" s="106"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
       <c r="T1" s="57" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F2" s="106" t="s">
+      <c r="F2" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="106"/>
+      <c r="G2" s="107"/>
       <c r="H2">
         <v>53</v>
       </c>
@@ -2186,11 +2186,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="107" t="s">
+      <c r="B20" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2229,10 +2229,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="G2" s="106" t="s">
+      <c r="G2" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="106"/>
+      <c r="H2" s="107"/>
       <c r="I2">
         <v>19</v>
       </c>
@@ -2710,10 +2710,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="106" t="s">
+      <c r="E2" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="106"/>
+      <c r="F2" s="107"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -3155,7 +3155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R7" activeCellId="1" sqref="S5:T11 R7:R9"/>
     </sheetView>
   </sheetViews>
@@ -3171,10 +3171,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="106" t="s">
+      <c r="E2" s="107" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="106"/>
+      <c r="F2" s="107"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -3367,7 +3367,7 @@
       <c r="S8" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="T8" s="108" t="s">
+      <c r="T8" s="106" t="s">
         <v>102</v>
       </c>
       <c r="U8" s="2"/>
@@ -3403,7 +3403,7 @@
       <c r="R9" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="S9" s="108" t="s">
+      <c r="S9" s="106" t="s">
         <v>110</v>
       </c>
       <c r="T9" s="94" t="s">

</xml_diff>

<commit_message>
Change lay out for all rooms to more desirable colors and empty rules
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -776,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -972,9 +972,6 @@
     <xf numFmtId="1" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -997,9 +994,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1420,7 +1414,7 @@
   <dimension ref="A1:AG20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4:Z7"/>
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,20 +1427,20 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="107" t="s">
+      <c r="Q1" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
       <c r="T1" s="57" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="107"/>
+      <c r="G2" s="105"/>
       <c r="H2">
         <v>53</v>
       </c>
@@ -1515,23 +1509,23 @@
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="12"/>
-      <c r="R4" s="70" t="str">
+      <c r="R4" s="69" t="str">
         <f>CONCATENATE(R15,N4,)</f>
         <v>0411</v>
       </c>
-      <c r="S4" s="70" t="str">
+      <c r="S4" s="69" t="str">
         <f>CONCATENATE(S15,N4,)</f>
         <v>0511</v>
       </c>
-      <c r="T4" s="70" t="str">
+      <c r="T4" s="69" t="str">
         <f>CONCATENATE(T15,N4)</f>
         <v>0611</v>
       </c>
-      <c r="U4" s="70" t="str">
+      <c r="U4" s="69" t="str">
         <f>CONCATENATE(U15,N4)</f>
         <v>0711</v>
       </c>
-      <c r="V4" s="70" t="str">
+      <c r="V4" s="69" t="str">
         <f>CONCATENATE(V15,N4)</f>
         <v>0811</v>
       </c>
@@ -1578,19 +1572,19 @@
       <c r="O5" s="5"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="31"/>
-      <c r="R5" s="70" t="str">
+      <c r="R5" s="69" t="str">
         <f>CONCATENATE(R15,N5,)</f>
         <v>0410</v>
       </c>
-      <c r="S5" s="84" t="str">
+      <c r="S5" s="82" t="str">
         <f>CONCATENATE(S15,N5,)</f>
         <v>0510</v>
       </c>
-      <c r="T5" s="85" t="str">
+      <c r="T5" s="83" t="str">
         <f>CONCATENATE(T15,N5)</f>
         <v>0610</v>
       </c>
-      <c r="U5" s="86" t="str">
+      <c r="U5" s="84" t="str">
         <f>CONCATENATE(U15,N5)</f>
         <v>0710</v>
       </c>
@@ -1639,23 +1633,23 @@
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="70" t="str">
+      <c r="Q6" s="69" t="str">
         <f>CONCATENATE(Q15,N6,)</f>
         <v>0309</v>
       </c>
-      <c r="R6" s="70" t="str">
+      <c r="R6" s="69" t="str">
         <f>CONCATENATE(R15,N6,)</f>
         <v>0409</v>
       </c>
-      <c r="S6" s="87" t="str">
+      <c r="S6" s="85" t="str">
         <f>CONCATENATE(S15,N6,)</f>
         <v>0509</v>
       </c>
-      <c r="T6" s="71" t="str">
+      <c r="T6" s="70" t="str">
         <f>CONCATENATE(T15,N6)</f>
         <v>0609</v>
       </c>
-      <c r="U6" s="88" t="str">
+      <c r="U6" s="86" t="str">
         <f>CONCATENATE(U15,N6)</f>
         <v>0709</v>
       </c>
@@ -1704,23 +1698,23 @@
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="14"/>
-      <c r="Q7" s="70" t="str">
+      <c r="Q7" s="69" t="str">
         <f>CONCATENATE(Q15,N7,)</f>
         <v>0308</v>
       </c>
-      <c r="R7" s="77" t="str">
+      <c r="R7" s="75" t="str">
         <f>CONCATENATE(R15,N7,)</f>
         <v>0408</v>
       </c>
-      <c r="S7" s="74" t="str">
+      <c r="S7" s="73" t="str">
         <f>CONCATENATE(S15,N7)</f>
         <v>0508</v>
       </c>
-      <c r="T7" s="72" t="str">
+      <c r="T7" s="71" t="str">
         <f>CONCATENATE(T15,N7)</f>
         <v>0608</v>
       </c>
-      <c r="U7" s="76" t="str">
+      <c r="U7" s="80" t="str">
         <f>CONCATENATE(U15,N7)</f>
         <v>0708</v>
       </c>
@@ -1769,35 +1763,35 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="14"/>
-      <c r="Q8" s="70" t="str">
+      <c r="Q8" s="69" t="str">
         <f>CONCATENATE(Q15,N8,)</f>
         <v>0307</v>
       </c>
-      <c r="R8" s="78" t="str">
+      <c r="R8" s="76" t="str">
         <f>CONCATENATE(R15,N8,)</f>
         <v>0407</v>
       </c>
-      <c r="S8" s="73" t="str">
+      <c r="S8" s="72" t="str">
         <f>CONCATENATE(S15,N8)</f>
         <v>0507</v>
       </c>
-      <c r="T8" s="73" t="str">
+      <c r="T8" s="72" t="str">
         <f>CONCATENATE(T15,N8)</f>
         <v>0607</v>
       </c>
-      <c r="U8" s="69" t="str">
+      <c r="U8" s="68" t="str">
         <f>CONCATENATE(U15,N8)</f>
         <v>0707</v>
       </c>
-      <c r="V8" s="72" t="str">
+      <c r="V8" s="71" t="str">
         <f>CONCATENATE(V15,N8)</f>
         <v>0807</v>
       </c>
-      <c r="W8" s="67" t="str">
+      <c r="W8" s="71" t="str">
         <f>CONCATENATE(W15,N8)</f>
         <v>0907</v>
       </c>
-      <c r="X8" s="6"/>
+      <c r="X8" s="5"/>
       <c r="Z8" s="58"/>
       <c r="AG8" s="6"/>
     </row>
@@ -1835,23 +1829,23 @@
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="72" t="str">
+      <c r="Q9" s="71" t="str">
         <f>CONCATENATE(Q15,N9,)</f>
         <v>0306</v>
       </c>
-      <c r="R9" s="79" t="str">
+      <c r="R9" s="77" t="str">
         <f>CONCATENATE(R15,N9,)</f>
         <v>0406</v>
       </c>
-      <c r="S9" s="69" t="str">
+      <c r="S9" s="68" t="str">
         <f>CONCATENATE(S15,N9)</f>
         <v>0506</v>
       </c>
-      <c r="T9" s="75" t="str">
+      <c r="T9" s="74" t="str">
         <f>CONCATENATE(T15,N9)</f>
         <v>0606</v>
       </c>
-      <c r="U9" s="82" t="str">
+      <c r="U9" s="80" t="str">
         <f>CONCATENATE(U15,N9)</f>
         <v>0706</v>
       </c>
@@ -1898,19 +1892,19 @@
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="69" t="str">
+      <c r="Q10" s="68" t="str">
         <f>CONCATENATE(Q15,N10,)</f>
         <v>0305</v>
       </c>
-      <c r="R10" s="70" t="str">
+      <c r="R10" s="69" t="str">
         <f>CONCATENATE(R15,N10,)</f>
         <v>0405</v>
       </c>
-      <c r="S10" s="80" t="str">
+      <c r="S10" s="78" t="str">
         <f>CONCATENATE(S15,N10)</f>
         <v>0505</v>
       </c>
-      <c r="T10" s="81" t="str">
+      <c r="T10" s="79" t="str">
         <f>CONCATENATE(T15,N10)</f>
         <v>0605</v>
       </c>
@@ -1960,19 +1954,19 @@
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="70" t="str">
+      <c r="R11" s="69" t="str">
         <f>CONCATENATE(R15,N11,)</f>
         <v>0404</v>
       </c>
-      <c r="S11" s="83" t="str">
+      <c r="S11" s="81" t="str">
         <f>CONCATENATE(S15,N11)</f>
         <v>0504</v>
       </c>
-      <c r="T11" s="69" t="str">
+      <c r="T11" s="68" t="str">
         <f>CONCATENATE(T15,N11)</f>
         <v>0604</v>
       </c>
-      <c r="U11" s="68" t="str">
+      <c r="U11" s="67" t="str">
         <f>CONCATENATE(U15,N11)</f>
         <v>0704</v>
       </c>
@@ -2018,27 +2012,27 @@
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="12"/>
-      <c r="R12" s="69" t="str">
+      <c r="R12" s="68" t="str">
         <f>CONCATENATE(R15,N12,)</f>
         <v>0403</v>
       </c>
-      <c r="S12" s="69" t="str">
+      <c r="S12" s="68" t="str">
         <f>CONCATENATE(S15,N12)</f>
         <v>0503</v>
       </c>
-      <c r="T12" s="69" t="str">
+      <c r="T12" s="68" t="str">
         <f>CONCATENATE(T15,N12)</f>
         <v>0603</v>
       </c>
-      <c r="U12" s="69" t="str">
+      <c r="U12" s="68" t="str">
         <f>CONCATENATE(U15,N12)</f>
         <v>0703</v>
       </c>
-      <c r="V12" s="69" t="str">
+      <c r="V12" s="68" t="str">
         <f>CONCATENATE(V15,N12)</f>
         <v>0803</v>
       </c>
-      <c r="W12" s="68" t="str">
+      <c r="W12" s="67" t="str">
         <f>CONCATENATE(W15,N12)</f>
         <v>0903</v>
       </c>
@@ -2186,11 +2180,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="108"/>
-      <c r="D20" s="108"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2229,10 +2223,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="G2" s="107" t="s">
+      <c r="G2" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="107"/>
+      <c r="H2" s="105"/>
       <c r="I2">
         <v>19</v>
       </c>
@@ -2311,11 +2305,11 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="90"/>
-      <c r="S5" s="91" t="s">
+      <c r="R5" s="88"/>
+      <c r="S5" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="T5" s="92" t="s">
+      <c r="T5" s="90" t="s">
         <v>99</v>
       </c>
       <c r="U5" s="22"/>
@@ -2347,11 +2341,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="95" t="s">
+      <c r="R6" s="88"/>
+      <c r="S6" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="T6" s="94" t="s">
+      <c r="T6" s="92" t="s">
         <v>100</v>
       </c>
       <c r="U6" s="22"/>
@@ -2366,7 +2360,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="89"/>
+      <c r="F7" s="87"/>
       <c r="G7" s="17" t="s">
         <v>49</v>
       </c>
@@ -2384,14 +2378,14 @@
       <c r="N7" s="5"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="89"/>
-      <c r="R7" s="98" t="s">
+      <c r="Q7" s="87"/>
+      <c r="R7" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="S7" s="96" t="s">
+      <c r="S7" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="T7" s="94" t="s">
+      <c r="T7" s="92" t="s">
         <v>101</v>
       </c>
       <c r="U7" s="22"/>
@@ -2406,7 +2400,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="89"/>
+      <c r="F8" s="87"/>
       <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
@@ -2424,14 +2418,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="89"/>
-      <c r="R8" s="93" t="s">
+      <c r="Q8" s="87"/>
+      <c r="R8" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="S8" s="96" t="s">
+      <c r="S8" s="94" t="s">
         <v>109</v>
       </c>
-      <c r="T8" s="97" t="s">
+      <c r="T8" s="95" t="s">
         <v>102</v>
       </c>
       <c r="U8" s="5"/>
@@ -2446,7 +2440,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="89"/>
+      <c r="F9" s="87"/>
       <c r="G9" s="28" t="s">
         <v>51</v>
       </c>
@@ -2464,14 +2458,14 @@
       <c r="N9" s="5"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="99" t="s">
+      <c r="Q9" s="87"/>
+      <c r="R9" s="97" t="s">
         <v>115</v>
       </c>
-      <c r="S9" s="101" t="s">
+      <c r="S9" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="T9" s="100" t="s">
+      <c r="T9" s="98" t="s">
         <v>103</v>
       </c>
       <c r="U9" s="22"/>
@@ -2502,13 +2496,13 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="98" t="s">
+      <c r="R10" s="96" t="s">
         <v>116</v>
       </c>
-      <c r="S10" s="93" t="s">
+      <c r="S10" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="T10" s="94" t="s">
+      <c r="T10" s="92" t="s">
         <v>104</v>
       </c>
       <c r="U10" s="22"/>
@@ -2539,13 +2533,13 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="99" t="s">
+      <c r="R11" s="97" t="s">
         <v>117</v>
       </c>
-      <c r="S11" s="95" t="s">
+      <c r="S11" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="T11" s="102" t="s">
+      <c r="T11" s="100" t="s">
         <v>105</v>
       </c>
       <c r="U11" s="22"/>
@@ -2710,10 +2704,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="107"/>
+      <c r="F2" s="105"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -2789,11 +2783,11 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="90"/>
-      <c r="S5" s="91" t="s">
+      <c r="R5" s="88"/>
+      <c r="S5" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="T5" s="92" t="s">
+      <c r="T5" s="90" t="s">
         <v>127</v>
       </c>
       <c r="U5" s="22"/>
@@ -2824,11 +2818,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="95" t="s">
+      <c r="R6" s="88"/>
+      <c r="S6" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="T6" s="94" t="s">
+      <c r="T6" s="92" t="s">
         <v>128</v>
       </c>
       <c r="U6" s="22"/>
@@ -2861,13 +2855,13 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="91" t="s">
+      <c r="R7" s="89" t="s">
         <v>134</v>
       </c>
-      <c r="S7" s="96" t="s">
+      <c r="S7" s="94" t="s">
         <v>122</v>
       </c>
-      <c r="T7" s="94" t="s">
+      <c r="T7" s="92" t="s">
         <v>129</v>
       </c>
       <c r="U7" s="22"/>
@@ -2900,13 +2894,13 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="93" t="s">
+      <c r="R8" s="91" t="s">
         <v>135</v>
       </c>
-      <c r="S8" s="105" t="s">
+      <c r="S8" s="103" t="s">
         <v>123</v>
       </c>
-      <c r="T8" s="97" t="s">
+      <c r="T8" s="95" t="s">
         <v>130</v>
       </c>
       <c r="U8" s="5"/>
@@ -2939,13 +2933,13 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="99" t="s">
+      <c r="R9" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="S9" s="101" t="s">
+      <c r="S9" s="99" t="s">
         <v>124</v>
       </c>
-      <c r="T9" s="94" t="s">
+      <c r="T9" s="92" t="s">
         <v>131</v>
       </c>
       <c r="U9" s="22"/>
@@ -2973,11 +2967,11 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="103"/>
-      <c r="S10" s="93" t="s">
+      <c r="R10" s="101"/>
+      <c r="S10" s="91" t="s">
         <v>125</v>
       </c>
-      <c r="T10" s="102" t="s">
+      <c r="T10" s="100" t="s">
         <v>132</v>
       </c>
       <c r="U10" s="22"/>
@@ -3005,11 +2999,11 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="95" t="s">
+      <c r="R11" s="102"/>
+      <c r="S11" s="93" t="s">
         <v>126</v>
       </c>
-      <c r="T11" s="102" t="s">
+      <c r="T11" s="100" t="s">
         <v>133</v>
       </c>
       <c r="U11" s="22"/>
@@ -3171,10 +3165,10 @@
       </c>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="107"/>
+      <c r="F2" s="105"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -3250,11 +3244,11 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="90"/>
-      <c r="S5" s="91" t="s">
+      <c r="R5" s="88"/>
+      <c r="S5" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="T5" s="92" t="s">
+      <c r="T5" s="90" t="s">
         <v>99</v>
       </c>
       <c r="U5" s="1"/>
@@ -3285,11 +3279,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="90"/>
-      <c r="S6" s="93" t="s">
+      <c r="R6" s="88"/>
+      <c r="S6" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="T6" s="94" t="s">
+      <c r="T6" s="92" t="s">
         <v>100</v>
       </c>
       <c r="U6" s="1"/>
@@ -3322,13 +3316,13 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="91" t="s">
+      <c r="R7" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="S7" s="96" t="s">
+      <c r="S7" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="T7" s="94" t="s">
+      <c r="T7" s="92" t="s">
         <v>101</v>
       </c>
       <c r="U7" s="1"/>
@@ -3361,13 +3355,13 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="93" t="s">
+      <c r="R8" s="91" t="s">
         <v>114</v>
       </c>
-      <c r="S8" s="96" t="s">
+      <c r="S8" s="94" t="s">
         <v>109</v>
       </c>
-      <c r="T8" s="106" t="s">
+      <c r="T8" s="104" t="s">
         <v>102</v>
       </c>
       <c r="U8" s="2"/>
@@ -3400,13 +3394,13 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="95" t="s">
+      <c r="R9" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="S9" s="106" t="s">
+      <c r="S9" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="T9" s="94" t="s">
+      <c r="T9" s="92" t="s">
         <v>103</v>
       </c>
       <c r="U9" s="1"/>
@@ -3434,11 +3428,11 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="103"/>
-      <c r="S10" s="93" t="s">
+      <c r="R10" s="101"/>
+      <c r="S10" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="T10" s="94" t="s">
+      <c r="T10" s="92" t="s">
         <v>104</v>
       </c>
       <c r="U10" s="1"/>
@@ -3466,11 +3460,11 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="95" t="s">
+      <c r="R11" s="102"/>
+      <c r="S11" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="T11" s="102" t="s">
+      <c r="T11" s="100" t="s">
         <v>105</v>
       </c>
       <c r="U11" s="1"/>

</xml_diff>

<commit_message>
Add locked doors to all applicable rooms
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="135">
   <si>
     <t>y/x</t>
   </si>
@@ -290,18 +290,6 @@
   </si>
   <si>
     <t>00</t>
-  </si>
-  <si>
-    <t>Nog niet in code</t>
-  </si>
-  <si>
-    <t>Kamer aangemaakt</t>
-  </si>
-  <si>
-    <t>Exits kloppen</t>
-  </si>
-  <si>
-    <t>Beschrijving volledig</t>
   </si>
   <si>
     <t>SSD1</t>
@@ -462,18 +450,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -483,31 +465,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -796,7 +754,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -814,9 +772,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -844,7 +799,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -856,9 +811,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,9 +821,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -887,210 +836,186 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1411,72 +1336,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG20"/>
+  <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="18" max="18" width="7.42578125" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" style="47" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="105" t="s">
+      <c r="Q1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="57" t="s">
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="53" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="F2" s="105" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="105"/>
+      <c r="G2" s="58"/>
       <c r="H2">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>12</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="N3" s="54">
+      <c r="N3" s="50">
         <v>12</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
-      <c r="V3" s="18"/>
-      <c r="W3" s="18"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
       <c r="X3" s="6"/>
-      <c r="Z3" s="58"/>
-      <c r="AG3" s="6"/>
-    </row>
-    <row r="4" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF3" s="6"/>
+    </row>
+    <row r="4" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>11</v>
       </c>
@@ -1498,207 +1421,198 @@
       <c r="I4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="N4" s="54">
+      <c r="N4" s="50">
         <v>11</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="69" t="str">
+      <c r="Q4" s="67"/>
+      <c r="R4" s="68" t="str">
         <f>CONCATENATE(R15,N4,)</f>
         <v>0411</v>
       </c>
-      <c r="S4" s="69" t="str">
+      <c r="S4" s="68" t="str">
         <f>CONCATENATE(S15,N4,)</f>
         <v>0511</v>
       </c>
-      <c r="T4" s="69" t="str">
+      <c r="T4" s="68" t="str">
         <f>CONCATENATE(T15,N4)</f>
         <v>0611</v>
       </c>
-      <c r="U4" s="69" t="str">
+      <c r="U4" s="68" t="str">
         <f>CONCATENATE(U15,N4)</f>
         <v>0711</v>
       </c>
-      <c r="V4" s="69" t="str">
+      <c r="V4" s="68" t="str">
         <f>CONCATENATE(V15,N4)</f>
         <v>0811</v>
       </c>
-      <c r="W4" s="66" t="str">
+      <c r="W4" s="67" t="str">
         <f>CONCATENATE(W15,N4)</f>
         <v>0911</v>
       </c>
       <c r="X4" s="6"/>
-      <c r="Z4" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG4" s="6"/>
-    </row>
-    <row r="5" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF4" s="6"/>
+    </row>
+    <row r="5" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="31"/>
+      <c r="D5" s="29"/>
       <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="H5" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="I5" s="27" t="s">
+      <c r="F5" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="N5" s="54">
+      <c r="N5" s="50">
         <v>10</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="31"/>
-      <c r="R5" s="69" t="str">
+      <c r="Q5" s="69"/>
+      <c r="R5" s="68" t="str">
         <f>CONCATENATE(R15,N5,)</f>
         <v>0410</v>
       </c>
-      <c r="S5" s="82" t="str">
+      <c r="S5" s="70" t="str">
         <f>CONCATENATE(S15,N5,)</f>
         <v>0510</v>
       </c>
-      <c r="T5" s="83" t="str">
+      <c r="T5" s="71" t="str">
         <f>CONCATENATE(T15,N5)</f>
         <v>0610</v>
       </c>
-      <c r="U5" s="84" t="str">
+      <c r="U5" s="72" t="str">
         <f>CONCATENATE(U15,N5)</f>
         <v>0710</v>
       </c>
-      <c r="V5" s="63"/>
-      <c r="W5" s="66" t="str">
+      <c r="V5" s="54"/>
+      <c r="W5" s="67" t="str">
         <f>CONCATENATE(W15,N5)</f>
         <v>0910</v>
       </c>
       <c r="X5" s="6"/>
-      <c r="Z5" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="AG5" s="6"/>
-    </row>
-    <row r="6" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF5" s="6"/>
+    </row>
+    <row r="6" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="14"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="G6" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>98</v>
-      </c>
-      <c r="I6" s="13" t="s">
+      <c r="F6" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="N6" s="54" t="s">
+      <c r="N6" s="50" t="s">
         <v>86</v>
       </c>
       <c r="O6" s="5"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="69" t="str">
+      <c r="P6" s="13"/>
+      <c r="Q6" s="68" t="str">
         <f>CONCATENATE(Q15,N6,)</f>
         <v>0309</v>
       </c>
-      <c r="R6" s="69" t="str">
+      <c r="R6" s="68" t="str">
         <f>CONCATENATE(R15,N6,)</f>
         <v>0409</v>
       </c>
-      <c r="S6" s="85" t="str">
+      <c r="S6" s="73" t="str">
         <f>CONCATENATE(S15,N6,)</f>
         <v>0509</v>
       </c>
-      <c r="T6" s="70" t="str">
+      <c r="T6" s="66" t="str">
         <f>CONCATENATE(T15,N6)</f>
         <v>0609</v>
       </c>
-      <c r="U6" s="86" t="str">
+      <c r="U6" s="74" t="str">
         <f>CONCATENATE(U15,N6)</f>
         <v>0709</v>
       </c>
-      <c r="V6" s="64"/>
-      <c r="W6" s="66" t="str">
+      <c r="V6" s="55"/>
+      <c r="W6" s="67" t="str">
         <f>CONCATENATE(W15,N6)</f>
         <v>0909</v>
       </c>
       <c r="X6" s="6"/>
-      <c r="Z6" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="AG6" s="6"/>
-    </row>
-    <row r="7" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF6" s="6"/>
+    </row>
+    <row r="7" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>8</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="14"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="I7" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="N7" s="54" t="s">
+      <c r="N7" s="50" t="s">
         <v>85</v>
       </c>
       <c r="O7" s="5"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="69" t="str">
+      <c r="P7" s="13"/>
+      <c r="Q7" s="68" t="str">
         <f>CONCATENATE(Q15,N7,)</f>
         <v>0308</v>
       </c>
@@ -1706,39 +1620,36 @@
         <f>CONCATENATE(R15,N7,)</f>
         <v>0408</v>
       </c>
-      <c r="S7" s="73" t="str">
+      <c r="S7" s="76" t="str">
         <f>CONCATENATE(S15,N7)</f>
         <v>0508</v>
       </c>
-      <c r="T7" s="71" t="str">
+      <c r="T7" s="62" t="str">
         <f>CONCATENATE(T15,N7)</f>
         <v>0608</v>
       </c>
-      <c r="U7" s="80" t="str">
+      <c r="U7" s="77" t="str">
         <f>CONCATENATE(U15,N7)</f>
         <v>0708</v>
       </c>
-      <c r="V7" s="65"/>
-      <c r="W7" s="66" t="str">
+      <c r="V7" s="56"/>
+      <c r="W7" s="67" t="str">
         <f>CONCATENATE(W15,N7)</f>
         <v>0908</v>
       </c>
       <c r="X7" s="6"/>
-      <c r="Z7" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG7" s="6"/>
-    </row>
-    <row r="8" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF7" s="6"/>
+    </row>
+    <row r="8" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>18</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -1747,181 +1658,178 @@
       <c r="G8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="J8" s="40" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="N8" s="54" t="s">
+      <c r="N8" s="50" t="s">
         <v>84</v>
       </c>
       <c r="O8" s="5"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="69" t="str">
+      <c r="P8" s="13"/>
+      <c r="Q8" s="68" t="str">
         <f>CONCATENATE(Q15,N8,)</f>
         <v>0307</v>
       </c>
-      <c r="R8" s="76" t="str">
+      <c r="R8" s="65" t="str">
         <f>CONCATENATE(R15,N8,)</f>
         <v>0407</v>
       </c>
-      <c r="S8" s="72" t="str">
+      <c r="S8" s="78" t="str">
         <f>CONCATENATE(S15,N8)</f>
         <v>0507</v>
       </c>
-      <c r="T8" s="72" t="str">
+      <c r="T8" s="78" t="str">
         <f>CONCATENATE(T15,N8)</f>
         <v>0607</v>
       </c>
-      <c r="U8" s="68" t="str">
+      <c r="U8" s="64" t="str">
         <f>CONCATENATE(U15,N8)</f>
         <v>0707</v>
       </c>
-      <c r="V8" s="71" t="str">
+      <c r="V8" s="62" t="str">
         <f>CONCATENATE(V15,N8)</f>
         <v>0807</v>
       </c>
-      <c r="W8" s="71" t="str">
+      <c r="W8" s="62" t="str">
         <f>CONCATENATE(W15,N8)</f>
         <v>0907</v>
       </c>
       <c r="X8" s="5"/>
-      <c r="Z8" s="58"/>
-      <c r="AG8" s="6"/>
-    </row>
-    <row r="9" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF8" s="6"/>
+    </row>
+    <row r="9" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="24" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="N9" s="54" t="s">
+      <c r="N9" s="50" t="s">
         <v>83</v>
       </c>
       <c r="O9" s="5"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="71" t="str">
+      <c r="P9" s="13"/>
+      <c r="Q9" s="62" t="str">
         <f>CONCATENATE(Q15,N9,)</f>
         <v>0306</v>
       </c>
-      <c r="R9" s="77" t="str">
+      <c r="R9" s="63" t="str">
         <f>CONCATENATE(R15,N9,)</f>
         <v>0406</v>
       </c>
-      <c r="S9" s="68" t="str">
+      <c r="S9" s="64" t="str">
         <f>CONCATENATE(S15,N9)</f>
         <v>0506</v>
       </c>
-      <c r="T9" s="74" t="str">
+      <c r="T9" s="60" t="str">
         <f>CONCATENATE(T15,N9)</f>
         <v>0606</v>
       </c>
-      <c r="U9" s="80" t="str">
+      <c r="U9" s="77" t="str">
         <f>CONCATENATE(U15,N9)</f>
         <v>0706</v>
       </c>
-      <c r="V9" s="63"/>
-      <c r="W9" s="66" t="str">
+      <c r="V9" s="54"/>
+      <c r="W9" s="67" t="str">
         <f>CONCATENATE(W15,N9)</f>
         <v>0906</v>
       </c>
       <c r="X9" s="6"/>
-      <c r="Z9" s="58"/>
-      <c r="AG9" s="6"/>
-    </row>
-    <row r="10" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF9" s="6"/>
+    </row>
+    <row r="10" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="41" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="38" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="33" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-      <c r="N10" s="54" t="s">
+      <c r="N10" s="50" t="s">
         <v>82</v>
       </c>
       <c r="O10" s="5"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="68" t="str">
+      <c r="P10" s="13"/>
+      <c r="Q10" s="64" t="str">
         <f>CONCATENATE(Q15,N10,)</f>
         <v>0305</v>
       </c>
-      <c r="R10" s="69" t="str">
+      <c r="R10" s="68" t="str">
         <f>CONCATENATE(R15,N10,)</f>
         <v>0405</v>
       </c>
-      <c r="S10" s="78" t="str">
+      <c r="S10" s="79" t="str">
         <f>CONCATENATE(S15,N10)</f>
         <v>0505</v>
       </c>
-      <c r="T10" s="79" t="str">
+      <c r="T10" s="61" t="str">
         <f>CONCATENATE(T15,N10)</f>
         <v>0605</v>
       </c>
-      <c r="U10" s="66" t="str">
+      <c r="U10" s="67" t="str">
         <f>CONCATENATE(U15,N10)</f>
         <v>0705</v>
       </c>
-      <c r="V10" s="64"/>
-      <c r="W10" s="66" t="str">
+      <c r="V10" s="55"/>
+      <c r="W10" s="67" t="str">
         <f>CONCATENATE(W15,N10)</f>
         <v>0905</v>
       </c>
       <c r="X10" s="6"/>
-      <c r="Z10" s="58"/>
-      <c r="AG10" s="6"/>
-    </row>
-    <row r="11" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF10" s="6"/>
+    </row>
+    <row r="11" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1931,116 +1839,114 @@
       <c r="E11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="N11" s="54" t="s">
+      <c r="N11" s="50" t="s">
         <v>81</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="69" t="str">
+      <c r="Q11" s="67"/>
+      <c r="R11" s="68" t="str">
         <f>CONCATENATE(R15,N11,)</f>
         <v>0404</v>
       </c>
-      <c r="S11" s="81" t="str">
+      <c r="S11" s="80" t="str">
         <f>CONCATENATE(S15,N11)</f>
         <v>0504</v>
       </c>
-      <c r="T11" s="68" t="str">
+      <c r="T11" s="64" t="str">
         <f>CONCATENATE(T15,N11)</f>
         <v>0604</v>
       </c>
-      <c r="U11" s="67" t="str">
+      <c r="U11" s="69" t="str">
         <f>CONCATENATE(U15,N11)</f>
         <v>0704</v>
       </c>
-      <c r="V11" s="65"/>
-      <c r="W11" s="66" t="str">
+      <c r="V11" s="56"/>
+      <c r="W11" s="67" t="str">
         <f>CONCATENATE(W15,N11)</f>
         <v>0904</v>
       </c>
       <c r="X11" s="6"/>
-      <c r="Z11" s="58"/>
-      <c r="AG11" s="6"/>
-    </row>
-    <row r="12" spans="1:33" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF11" s="6"/>
+    </row>
+    <row r="12" spans="1:32" s="1" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="44" t="s">
+      <c r="E12" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="41" t="s">
         <v>9</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="N12" s="54" t="s">
+      <c r="N12" s="50" t="s">
         <v>80</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="68" t="str">
+      <c r="Q12" s="67"/>
+      <c r="R12" s="64" t="str">
         <f>CONCATENATE(R15,N12,)</f>
         <v>0403</v>
       </c>
-      <c r="S12" s="68" t="str">
+      <c r="S12" s="64" t="str">
         <f>CONCATENATE(S15,N12)</f>
         <v>0503</v>
       </c>
-      <c r="T12" s="68" t="str">
+      <c r="T12" s="64" t="str">
         <f>CONCATENATE(T15,N12)</f>
         <v>0603</v>
       </c>
-      <c r="U12" s="68" t="str">
+      <c r="U12" s="64" t="str">
         <f>CONCATENATE(U15,N12)</f>
         <v>0703</v>
       </c>
-      <c r="V12" s="68" t="str">
+      <c r="V12" s="64" t="str">
         <f>CONCATENATE(V15,N12)</f>
         <v>0803</v>
       </c>
-      <c r="W12" s="67" t="str">
+      <c r="W12" s="69" t="str">
         <f>CONCATENATE(W15,N12)</f>
         <v>0903</v>
       </c>
       <c r="X12" s="6"/>
-      <c r="Z12" s="58"/>
-      <c r="AG12" s="6"/>
-    </row>
-    <row r="13" spans="1:33" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF12" s="6"/>
+    </row>
+    <row r="13" spans="1:32" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -2054,8 +1960,8 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
-      <c r="L13" s="34"/>
-      <c r="N13" s="54" t="s">
+      <c r="L13" s="31"/>
+      <c r="N13" s="50" t="s">
         <v>79</v>
       </c>
       <c r="O13" s="5"/>
@@ -2068,39 +1974,39 @@
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
-      <c r="AG13" s="34"/>
-    </row>
-    <row r="14" spans="1:33" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF13" s="31"/>
+    </row>
+    <row r="14" spans="1:32" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="34"/>
-      <c r="N14" s="54" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="31"/>
+      <c r="N14" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="O14" s="29"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-      <c r="V14" s="18"/>
-      <c r="W14" s="18"/>
-      <c r="X14" s="18"/>
-      <c r="AG14" s="22"/>
-    </row>
-    <row r="15" spans="1:33" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="27"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="AF14" s="21"/>
+    </row>
+    <row r="15" spans="1:32" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2137,37 +2043,37 @@
       <c r="N15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O15" s="54" t="s">
+      <c r="O15" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="P15" s="54" t="s">
+      <c r="P15" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="Q15" s="54" t="s">
+      <c r="Q15" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="R15" s="55" t="s">
+      <c r="R15" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="S15" s="56" t="s">
+      <c r="S15" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="T15" s="56" t="s">
+      <c r="T15" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="U15" s="56" t="s">
+      <c r="U15" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="V15" s="56" t="s">
+      <c r="V15" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="W15" s="55" t="s">
+      <c r="W15" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="X15" s="54">
+      <c r="X15" s="50">
         <v>10</v>
       </c>
-      <c r="AG15" s="1"/>
+      <c r="AF15" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2180,11 +2086,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="106"/>
-      <c r="D20" s="106"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2203,10 +2109,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W15"/>
+  <dimension ref="B1:U15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5:W8"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,24 +2120,23 @@
     <col min="2" max="6" width="7.140625" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" customWidth="1"/>
     <col min="8" max="10" width="7.140625" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="G2" s="105" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="G2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="105"/>
+      <c r="H2" s="58"/>
       <c r="I2">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>12</v>
       </c>
@@ -2256,7 +2161,7 @@
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>11</v>
       </c>
@@ -2281,7 +2186,7 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
     </row>
-    <row r="5" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>10</v>
       </c>
@@ -2290,13 +2195,13 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="35" t="s">
-        <v>118</v>
+      <c r="H5" s="32" t="s">
+        <v>114</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="22"/>
+        <v>115</v>
+      </c>
+      <c r="J5" s="21"/>
       <c r="K5" s="6"/>
       <c r="M5" s="1">
         <v>10</v>
@@ -2305,19 +2210,16 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="T5" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="U5" s="22"/>
-      <c r="W5" s="60" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="81"/>
+      <c r="S5" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="T5" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="U5" s="21"/>
+    </row>
+    <row r="6" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>9</v>
       </c>
@@ -2326,13 +2228,13 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="22"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="6"/>
       <c r="M6" s="1">
         <v>9</v>
@@ -2341,36 +2243,33 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="88"/>
-      <c r="S6" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="T6" s="92" t="s">
-        <v>100</v>
-      </c>
-      <c r="U6" s="22"/>
-      <c r="W6" s="59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="81"/>
+      <c r="S6" s="88" t="s">
+        <v>103</v>
+      </c>
+      <c r="T6" s="85" t="s">
+        <v>96</v>
+      </c>
+      <c r="U6" s="21"/>
+    </row>
+    <row r="7" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="57"/>
+      <c r="G7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="22"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="6"/>
       <c r="M7" s="1">
         <v>8</v>
@@ -2378,79 +2277,73 @@
       <c r="N7" s="5"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="87"/>
-      <c r="R7" s="96" t="s">
-        <v>113</v>
-      </c>
-      <c r="S7" s="94" t="s">
-        <v>108</v>
-      </c>
-      <c r="T7" s="92" t="s">
-        <v>101</v>
-      </c>
-      <c r="U7" s="22"/>
-      <c r="W7" s="61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="57"/>
+      <c r="R7" s="94" t="s">
+        <v>109</v>
+      </c>
+      <c r="S7" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" s="85" t="s">
+        <v>97</v>
+      </c>
+      <c r="U7" s="21"/>
+    </row>
+    <row r="8" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="87"/>
+      <c r="F8" s="57"/>
       <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>56</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="22"/>
+      <c r="K8" s="21"/>
       <c r="M8" s="1">
         <v>7</v>
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="87"/>
-      <c r="R8" s="91" t="s">
-        <v>114</v>
-      </c>
-      <c r="S8" s="94" t="s">
-        <v>109</v>
-      </c>
-      <c r="T8" s="95" t="s">
-        <v>102</v>
+      <c r="Q8" s="57"/>
+      <c r="R8" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="S8" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="T8" s="91" t="s">
+        <v>98</v>
       </c>
       <c r="U8" s="5"/>
-      <c r="W8" s="62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="57"/>
+      <c r="G9" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="22"/>
+      <c r="J9" s="21"/>
       <c r="K9" s="6"/>
       <c r="M9" s="1">
         <v>6</v>
@@ -2458,19 +2351,19 @@
       <c r="N9" s="5"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="87"/>
-      <c r="R9" s="97" t="s">
-        <v>115</v>
-      </c>
-      <c r="S9" s="99" t="s">
-        <v>110</v>
-      </c>
-      <c r="T9" s="98" t="s">
-        <v>103</v>
-      </c>
-      <c r="U9" s="22"/>
-    </row>
-    <row r="10" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="57"/>
+      <c r="R9" s="92" t="s">
+        <v>111</v>
+      </c>
+      <c r="S9" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="T9" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="U9" s="21"/>
+    </row>
+    <row r="10" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -2478,16 +2371,16 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="35" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="6"/>
       <c r="M10" s="1">
         <v>5</v>
@@ -2496,18 +2389,18 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="96" t="s">
-        <v>116</v>
-      </c>
-      <c r="S10" s="91" t="s">
-        <v>111</v>
-      </c>
-      <c r="T10" s="92" t="s">
-        <v>104</v>
-      </c>
-      <c r="U10" s="22"/>
-    </row>
-    <row r="11" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="S10" s="84" t="s">
+        <v>107</v>
+      </c>
+      <c r="T10" s="85" t="s">
+        <v>100</v>
+      </c>
+      <c r="U10" s="21"/>
+    </row>
+    <row r="11" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -2515,16 +2408,16 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="22"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="6"/>
       <c r="M11" s="1">
         <v>4</v>
@@ -2533,18 +2426,18 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="97" t="s">
-        <v>117</v>
-      </c>
-      <c r="S11" s="93" t="s">
-        <v>112</v>
-      </c>
-      <c r="T11" s="100" t="s">
-        <v>105</v>
-      </c>
-      <c r="U11" s="22"/>
-    </row>
-    <row r="12" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="S11" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="T11" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="U11" s="21"/>
+    </row>
+    <row r="12" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -2569,57 +2462,57 @@
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
     </row>
-    <row r="13" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
       <c r="M13" s="1">
         <v>2</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-    </row>
-    <row r="14" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+    </row>
+    <row r="14" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="34"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="31"/>
       <c r="M14" s="1">
         <v>1</v>
       </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-    </row>
-    <row r="15" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="27"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+    </row>
+    <row r="15" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -2686,33 +2579,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W15"/>
+  <dimension ref="B1:U15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="10" width="7.140625" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="105" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="105"/>
+      <c r="F2" s="58"/>
       <c r="G2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>12</v>
       </c>
@@ -2736,7 +2628,7 @@
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
     </row>
-    <row r="4" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>11</v>
       </c>
@@ -2760,7 +2652,7 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
     </row>
-    <row r="5" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>10</v>
       </c>
@@ -2775,7 +2667,7 @@
       <c r="I5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="22"/>
+      <c r="J5" s="21"/>
       <c r="M5" s="1">
         <v>10</v>
       </c>
@@ -2783,19 +2675,16 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="89" t="s">
-        <v>120</v>
-      </c>
-      <c r="T5" s="90" t="s">
-        <v>127</v>
-      </c>
-      <c r="U5" s="22"/>
-      <c r="W5" s="60" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R5" s="81"/>
+      <c r="S5" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="T5" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="U5" s="21"/>
+    </row>
+    <row r="6" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>9</v>
       </c>
@@ -2804,13 +2693,13 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J6" s="22"/>
+      <c r="J6" s="21"/>
       <c r="M6" s="1">
         <v>9</v>
       </c>
@@ -2818,19 +2707,16 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="88"/>
-      <c r="S6" s="93" t="s">
-        <v>121</v>
-      </c>
-      <c r="T6" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="U6" s="22"/>
-      <c r="W6" s="59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="81"/>
+      <c r="S6" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="T6" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="U6" s="21"/>
+    </row>
+    <row r="7" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8</v>
       </c>
@@ -2841,13 +2727,13 @@
       <c r="G7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="22"/>
+      <c r="J7" s="21"/>
       <c r="M7" s="1">
         <v>8</v>
       </c>
@@ -2855,21 +2741,18 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="89" t="s">
-        <v>134</v>
-      </c>
-      <c r="S7" s="94" t="s">
-        <v>122</v>
-      </c>
-      <c r="T7" s="92" t="s">
-        <v>129</v>
-      </c>
-      <c r="U7" s="22"/>
-      <c r="W7" s="61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="82" t="s">
+        <v>130</v>
+      </c>
+      <c r="S7" s="86" t="s">
+        <v>118</v>
+      </c>
+      <c r="T7" s="85" t="s">
+        <v>125</v>
+      </c>
+      <c r="U7" s="21"/>
+    </row>
+    <row r="8" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -2880,10 +2763,10 @@
       <c r="G8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="19" t="s">
         <v>60</v>
       </c>
       <c r="J8" s="5"/>
@@ -2894,21 +2777,18 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="91" t="s">
-        <v>135</v>
-      </c>
-      <c r="S8" s="103" t="s">
-        <v>123</v>
-      </c>
-      <c r="T8" s="95" t="s">
-        <v>130</v>
+      <c r="R8" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="S8" s="90" t="s">
+        <v>119</v>
+      </c>
+      <c r="T8" s="91" t="s">
+        <v>126</v>
       </c>
       <c r="U8" s="5"/>
-      <c r="W8" s="62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -2916,16 +2796,16 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="22"/>
+      <c r="J9" s="21"/>
       <c r="M9" s="1">
         <v>6</v>
       </c>
@@ -2933,18 +2813,18 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="S9" s="99" t="s">
-        <v>124</v>
-      </c>
-      <c r="T9" s="92" t="s">
-        <v>131</v>
-      </c>
-      <c r="U9" s="22"/>
-    </row>
-    <row r="10" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="92" t="s">
+        <v>132</v>
+      </c>
+      <c r="S9" s="93" t="s">
+        <v>120</v>
+      </c>
+      <c r="T9" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="U9" s="21"/>
+    </row>
+    <row r="10" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -2956,10 +2836,10 @@
       <c r="H10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="21"/>
       <c r="M10" s="1">
         <v>5</v>
       </c>
@@ -2967,16 +2847,16 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="101"/>
-      <c r="S10" s="91" t="s">
-        <v>125</v>
-      </c>
-      <c r="T10" s="100" t="s">
-        <v>132</v>
-      </c>
-      <c r="U10" s="22"/>
-    </row>
-    <row r="11" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="83"/>
+      <c r="S10" s="84" t="s">
+        <v>121</v>
+      </c>
+      <c r="T10" s="89" t="s">
+        <v>128</v>
+      </c>
+      <c r="U10" s="21"/>
+    </row>
+    <row r="11" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -2984,14 +2864,14 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="J11" s="22"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="J11" s="21"/>
       <c r="M11" s="1">
         <v>4</v>
       </c>
@@ -2999,21 +2879,21 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="102"/>
-      <c r="S11" s="93" t="s">
-        <v>126</v>
-      </c>
-      <c r="T11" s="100" t="s">
-        <v>133</v>
-      </c>
-      <c r="U11" s="22"/>
-    </row>
-    <row r="12" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="85"/>
+      <c r="S11" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="T11" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="U11" s="21"/>
+    </row>
+    <row r="12" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>3</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="22"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -3024,7 +2904,7 @@
         <v>3</v>
       </c>
       <c r="N12" s="5"/>
-      <c r="O12" s="22"/>
+      <c r="O12" s="21"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
@@ -3032,55 +2912,55 @@
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
     </row>
-    <row r="13" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
       <c r="M13" s="1">
         <v>2</v>
       </c>
       <c r="N13" s="5"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="34"/>
-      <c r="U13" s="34"/>
-    </row>
-    <row r="14" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+    </row>
+    <row r="14" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
       <c r="M14" s="1">
         <v>1</v>
       </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-    </row>
-    <row r="15" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="27"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+    </row>
+    <row r="15" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -3147,33 +3027,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:W15"/>
+  <dimension ref="B1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R7" activeCellId="1" sqref="S5:T11 R7:R9"/>
+      <selection activeCell="R5" sqref="R5:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="10" width="7.140625" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="105" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E2" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="105"/>
+      <c r="F2" s="58"/>
       <c r="G2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>12</v>
       </c>
@@ -3197,7 +3076,7 @@
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>11</v>
       </c>
@@ -3221,7 +3100,7 @@
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>10</v>
       </c>
@@ -3244,19 +3123,16 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="T5" s="90" t="s">
-        <v>99</v>
+      <c r="R5" s="81"/>
+      <c r="S5" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="T5" s="83" t="s">
+        <v>95</v>
       </c>
       <c r="U5" s="1"/>
-      <c r="W5" s="60" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>9</v>
       </c>
@@ -3268,7 +3144,7 @@
       <c r="H6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>64</v>
       </c>
       <c r="J6" s="1"/>
@@ -3279,19 +3155,16 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="88"/>
-      <c r="S6" s="91" t="s">
-        <v>107</v>
-      </c>
-      <c r="T6" s="92" t="s">
-        <v>100</v>
+      <c r="R6" s="81"/>
+      <c r="S6" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="T6" s="85" t="s">
+        <v>96</v>
       </c>
       <c r="U6" s="1"/>
-      <c r="W6" s="59" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>8</v>
       </c>
@@ -3302,10 +3175,10 @@
       <c r="G7" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>67</v>
       </c>
       <c r="J7" s="1"/>
@@ -3316,21 +3189,18 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="89" t="s">
-        <v>113</v>
-      </c>
-      <c r="S7" s="94" t="s">
-        <v>108</v>
-      </c>
-      <c r="T7" s="92" t="s">
-        <v>101</v>
+      <c r="R7" s="82" t="s">
+        <v>109</v>
+      </c>
+      <c r="S7" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" s="85" t="s">
+        <v>97</v>
       </c>
       <c r="U7" s="1"/>
-      <c r="W7" s="61" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>7</v>
       </c>
@@ -3341,10 +3211,10 @@
       <c r="G8" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>70</v>
       </c>
       <c r="J8" s="2"/>
@@ -3355,21 +3225,18 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="91" t="s">
-        <v>114</v>
-      </c>
-      <c r="S8" s="94" t="s">
-        <v>109</v>
-      </c>
-      <c r="T8" s="104" t="s">
-        <v>102</v>
+      <c r="R8" s="84" t="s">
+        <v>110</v>
+      </c>
+      <c r="S8" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="T8" s="87" t="s">
+        <v>98</v>
       </c>
       <c r="U8" s="2"/>
-      <c r="W8" s="62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -3377,13 +3244,13 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>73</v>
       </c>
       <c r="J9" s="1"/>
@@ -3394,18 +3261,18 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="93" t="s">
-        <v>115</v>
-      </c>
-      <c r="S9" s="104" t="s">
-        <v>110</v>
-      </c>
-      <c r="T9" s="92" t="s">
-        <v>103</v>
+      <c r="R9" s="88" t="s">
+        <v>111</v>
+      </c>
+      <c r="S9" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="T9" s="85" t="s">
+        <v>99</v>
       </c>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -3417,7 +3284,7 @@
       <c r="H10" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>74</v>
       </c>
       <c r="J10" s="1"/>
@@ -3428,16 +3295,16 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="101"/>
-      <c r="S10" s="91" t="s">
-        <v>111</v>
-      </c>
-      <c r="T10" s="92" t="s">
-        <v>104</v>
+      <c r="R10" s="83"/>
+      <c r="S10" s="84" t="s">
+        <v>107</v>
+      </c>
+      <c r="T10" s="85" t="s">
+        <v>100</v>
       </c>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>4</v>
       </c>
@@ -3445,11 +3312,11 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="29" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="30" t="s">
         <v>75</v>
       </c>
       <c r="J11" s="1"/>
@@ -3460,16 +3327,16 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="102"/>
-      <c r="S11" s="93" t="s">
-        <v>112</v>
-      </c>
-      <c r="T11" s="100" t="s">
-        <v>105</v>
+      <c r="R11" s="85"/>
+      <c r="S11" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="T11" s="89" t="s">
+        <v>101</v>
       </c>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>3</v>
       </c>
@@ -3493,49 +3360,49 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
       <c r="M13" s="1">
         <v>2</v>
       </c>
       <c r="N13" s="5"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-    </row>
-    <row r="14" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+    </row>
+    <row r="14" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
       <c r="M14" s="1">
         <v>1</v>
       </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
-    </row>
-    <row r="15" spans="2:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N14" s="27"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+    </row>
+    <row r="15" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add ActionMessages to all rooms on first floor
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -13,6 +13,7 @@
     <sheet name="Fourth floor" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -292,24 +293,6 @@
     <t>00</t>
   </si>
   <si>
-    <t>SSD1</t>
-  </si>
-  <si>
-    <t>SSD2</t>
-  </si>
-  <si>
-    <t>SSD3</t>
-  </si>
-  <si>
-    <t>SSD4</t>
-  </si>
-  <si>
-    <t>SSD5</t>
-  </si>
-  <si>
-    <t>SSD6</t>
-  </si>
-  <si>
     <t>0710</t>
   </si>
   <si>
@@ -428,6 +411,27 @@
   </si>
   <si>
     <t>Castor</t>
+  </si>
+  <si>
+    <t>Vega</t>
+  </si>
+  <si>
+    <t>Rigel
+Polaris</t>
+  </si>
+  <si>
+    <t>Morpho</t>
+  </si>
+  <si>
+    <t>Antaris
+Mimosa</t>
+  </si>
+  <si>
+    <t>Entree
+SSD</t>
+  </si>
+  <si>
+    <t>Coord.</t>
   </si>
 </sst>
 </file>
@@ -903,119 +907,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1339,7 +1343,7 @@
   <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,20 +1355,20 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
       <c r="T1" s="53" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="58"/>
+      <c r="G2" s="94"/>
       <c r="H2">
         <v>53</v>
       </c>
@@ -1431,28 +1435,28 @@
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="68" t="str">
+      <c r="Q4" s="65"/>
+      <c r="R4" s="66" t="str">
         <f>CONCATENATE(R15,N4,)</f>
         <v>0411</v>
       </c>
-      <c r="S4" s="68" t="str">
+      <c r="S4" s="66" t="str">
         <f>CONCATENATE(S15,N4,)</f>
         <v>0511</v>
       </c>
-      <c r="T4" s="68" t="str">
+      <c r="T4" s="66" t="str">
         <f>CONCATENATE(T15,N4)</f>
         <v>0611</v>
       </c>
-      <c r="U4" s="68" t="str">
+      <c r="U4" s="66" t="str">
         <f>CONCATENATE(U15,N4)</f>
         <v>0711</v>
       </c>
-      <c r="V4" s="68" t="str">
+      <c r="V4" s="66" t="str">
         <f>CONCATENATE(V15,N4)</f>
         <v>0811</v>
       </c>
-      <c r="W4" s="67" t="str">
+      <c r="W4" s="65" t="str">
         <f>CONCATENATE(W15,N4)</f>
         <v>0911</v>
       </c>
@@ -1470,13 +1474,13 @@
         <v>9</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="H5" s="48" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="I5" s="54" t="s">
         <v>8</v>
@@ -1491,25 +1495,25 @@
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="68" t="str">
+      <c r="Q5" s="67"/>
+      <c r="R5" s="66" t="str">
         <f>CONCATENATE(R15,N5,)</f>
         <v>0410</v>
       </c>
-      <c r="S5" s="70" t="str">
+      <c r="S5" s="68" t="str">
         <f>CONCATENATE(S15,N5,)</f>
         <v>0510</v>
       </c>
-      <c r="T5" s="71" t="str">
+      <c r="T5" s="69" t="str">
         <f>CONCATENATE(T15,N5)</f>
         <v>0610</v>
       </c>
-      <c r="U5" s="72" t="str">
+      <c r="U5" s="70" t="str">
         <f>CONCATENATE(U15,N5)</f>
         <v>0710</v>
       </c>
       <c r="V5" s="54"/>
-      <c r="W5" s="67" t="str">
+      <c r="W5" s="65" t="str">
         <f>CONCATENATE(W15,N5)</f>
         <v>0910</v>
       </c>
@@ -1529,13 +1533,13 @@
         <v>9</v>
       </c>
       <c r="F6" s="45" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="H6" s="49" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="I6" s="55" t="s">
         <v>8</v>
@@ -1550,28 +1554,28 @@
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="13"/>
-      <c r="Q6" s="68" t="str">
+      <c r="Q6" s="66" t="str">
         <f>CONCATENATE(Q15,N6,)</f>
         <v>0309</v>
       </c>
-      <c r="R6" s="68" t="str">
+      <c r="R6" s="66" t="str">
         <f>CONCATENATE(R15,N6,)</f>
         <v>0409</v>
       </c>
-      <c r="S6" s="73" t="str">
+      <c r="S6" s="71" t="str">
         <f>CONCATENATE(S15,N6,)</f>
         <v>0509</v>
       </c>
-      <c r="T6" s="66" t="str">
+      <c r="T6" s="64" t="str">
         <f>CONCATENATE(T15,N6)</f>
         <v>0609</v>
       </c>
-      <c r="U6" s="74" t="str">
+      <c r="U6" s="72" t="str">
         <f>CONCATENATE(U15,N6)</f>
         <v>0709</v>
       </c>
       <c r="V6" s="55"/>
-      <c r="W6" s="67" t="str">
+      <c r="W6" s="65" t="str">
         <f>CONCATENATE(W15,N6)</f>
         <v>0909</v>
       </c>
@@ -1612,28 +1616,28 @@
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="13"/>
-      <c r="Q7" s="68" t="str">
+      <c r="Q7" s="66" t="str">
         <f>CONCATENATE(Q15,N7,)</f>
         <v>0308</v>
       </c>
-      <c r="R7" s="75" t="str">
+      <c r="R7" s="73" t="str">
         <f>CONCATENATE(R15,N7,)</f>
         <v>0408</v>
       </c>
-      <c r="S7" s="76" t="str">
+      <c r="S7" s="74" t="str">
         <f>CONCATENATE(S15,N7)</f>
         <v>0508</v>
       </c>
-      <c r="T7" s="62" t="str">
+      <c r="T7" s="60" t="str">
         <f>CONCATENATE(T15,N7)</f>
         <v>0608</v>
       </c>
-      <c r="U7" s="77" t="str">
+      <c r="U7" s="75" t="str">
         <f>CONCATENATE(U15,N7)</f>
         <v>0708</v>
       </c>
       <c r="V7" s="56"/>
-      <c r="W7" s="67" t="str">
+      <c r="W7" s="65" t="str">
         <f>CONCATENATE(W15,N7)</f>
         <v>0908</v>
       </c>
@@ -1674,31 +1678,31 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="13"/>
-      <c r="Q8" s="68" t="str">
+      <c r="Q8" s="66" t="str">
         <f>CONCATENATE(Q15,N8,)</f>
         <v>0307</v>
       </c>
-      <c r="R8" s="65" t="str">
+      <c r="R8" s="63" t="str">
         <f>CONCATENATE(R15,N8,)</f>
         <v>0407</v>
       </c>
-      <c r="S8" s="78" t="str">
+      <c r="S8" s="76" t="str">
         <f>CONCATENATE(S15,N8)</f>
         <v>0507</v>
       </c>
-      <c r="T8" s="78" t="str">
+      <c r="T8" s="76" t="str">
         <f>CONCATENATE(T15,N8)</f>
         <v>0607</v>
       </c>
-      <c r="U8" s="64" t="str">
+      <c r="U8" s="62" t="str">
         <f>CONCATENATE(U15,N8)</f>
         <v>0707</v>
       </c>
-      <c r="V8" s="62" t="str">
+      <c r="V8" s="60" t="str">
         <f>CONCATENATE(V15,N8)</f>
         <v>0807</v>
       </c>
-      <c r="W8" s="62" t="str">
+      <c r="W8" s="60" t="str">
         <f>CONCATENATE(W15,N8)</f>
         <v>0907</v>
       </c>
@@ -1739,28 +1743,28 @@
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="13"/>
-      <c r="Q9" s="62" t="str">
+      <c r="Q9" s="60" t="str">
         <f>CONCATENATE(Q15,N9,)</f>
         <v>0306</v>
       </c>
-      <c r="R9" s="63" t="str">
+      <c r="R9" s="61" t="str">
         <f>CONCATENATE(R15,N9,)</f>
         <v>0406</v>
       </c>
-      <c r="S9" s="64" t="str">
+      <c r="S9" s="62" t="str">
         <f>CONCATENATE(S15,N9)</f>
         <v>0506</v>
       </c>
-      <c r="T9" s="60" t="str">
+      <c r="T9" s="58" t="str">
         <f>CONCATENATE(T15,N9)</f>
         <v>0606</v>
       </c>
-      <c r="U9" s="77" t="str">
+      <c r="U9" s="75" t="str">
         <f>CONCATENATE(U15,N9)</f>
         <v>0706</v>
       </c>
       <c r="V9" s="54"/>
-      <c r="W9" s="67" t="str">
+      <c r="W9" s="65" t="str">
         <f>CONCATENATE(W15,N9)</f>
         <v>0906</v>
       </c>
@@ -1801,28 +1805,28 @@
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="13"/>
-      <c r="Q10" s="64" t="str">
+      <c r="Q10" s="62" t="str">
         <f>CONCATENATE(Q15,N10,)</f>
         <v>0305</v>
       </c>
-      <c r="R10" s="68" t="str">
+      <c r="R10" s="66" t="str">
         <f>CONCATENATE(R15,N10,)</f>
         <v>0405</v>
       </c>
-      <c r="S10" s="79" t="str">
+      <c r="S10" s="77" t="str">
         <f>CONCATENATE(S15,N10)</f>
         <v>0505</v>
       </c>
-      <c r="T10" s="61" t="str">
+      <c r="T10" s="59" t="str">
         <f>CONCATENATE(T15,N10)</f>
         <v>0605</v>
       </c>
-      <c r="U10" s="67" t="str">
+      <c r="U10" s="65" t="str">
         <f>CONCATENATE(U15,N10)</f>
         <v>0705</v>
       </c>
       <c r="V10" s="55"/>
-      <c r="W10" s="67" t="str">
+      <c r="W10" s="65" t="str">
         <f>CONCATENATE(W15,N10)</f>
         <v>0905</v>
       </c>
@@ -1861,25 +1865,25 @@
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="68" t="str">
+      <c r="Q11" s="65"/>
+      <c r="R11" s="66" t="str">
         <f>CONCATENATE(R15,N11,)</f>
         <v>0404</v>
       </c>
-      <c r="S11" s="80" t="str">
+      <c r="S11" s="78" t="str">
         <f>CONCATENATE(S15,N11)</f>
         <v>0504</v>
       </c>
-      <c r="T11" s="64" t="str">
+      <c r="T11" s="62" t="str">
         <f>CONCATENATE(T15,N11)</f>
         <v>0604</v>
       </c>
-      <c r="U11" s="69" t="str">
+      <c r="U11" s="67" t="str">
         <f>CONCATENATE(U15,N11)</f>
         <v>0704</v>
       </c>
       <c r="V11" s="56"/>
-      <c r="W11" s="67" t="str">
+      <c r="W11" s="65" t="str">
         <f>CONCATENATE(W15,N11)</f>
         <v>0904</v>
       </c>
@@ -1918,28 +1922,28 @@
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="67"/>
-      <c r="R12" s="64" t="str">
+      <c r="Q12" s="65"/>
+      <c r="R12" s="62" t="str">
         <f>CONCATENATE(R15,N12,)</f>
         <v>0403</v>
       </c>
-      <c r="S12" s="64" t="str">
+      <c r="S12" s="62" t="str">
         <f>CONCATENATE(S15,N12)</f>
         <v>0503</v>
       </c>
-      <c r="T12" s="64" t="str">
+      <c r="T12" s="62" t="str">
         <f>CONCATENATE(T15,N12)</f>
         <v>0603</v>
       </c>
-      <c r="U12" s="64" t="str">
+      <c r="U12" s="62" t="str">
         <f>CONCATENATE(U15,N12)</f>
         <v>0703</v>
       </c>
-      <c r="V12" s="64" t="str">
+      <c r="V12" s="62" t="str">
         <f>CONCATENATE(V15,N12)</f>
         <v>0803</v>
       </c>
-      <c r="W12" s="69" t="str">
+      <c r="W12" s="67" t="str">
         <f>CONCATENATE(W15,N12)</f>
         <v>0903</v>
       </c>
@@ -2086,11 +2090,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2128,10 +2132,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="58"/>
+      <c r="H2" s="94"/>
       <c r="I2">
         <v>19</v>
       </c>
@@ -2196,10 +2200,10 @@
       <c r="F5" s="1"/>
       <c r="G5" s="6"/>
       <c r="H5" s="32" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="6"/>
@@ -2210,12 +2214,12 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="T5" s="83" t="s">
-        <v>95</v>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="T5" s="81" t="s">
+        <v>89</v>
       </c>
       <c r="U5" s="21"/>
     </row>
@@ -2243,12 +2247,12 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="88" t="s">
-        <v>103</v>
-      </c>
-      <c r="T6" s="85" t="s">
-        <v>96</v>
+      <c r="R6" s="79"/>
+      <c r="S6" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="T6" s="83" t="s">
+        <v>90</v>
       </c>
       <c r="U6" s="21"/>
     </row>
@@ -2278,14 +2282,14 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="57"/>
-      <c r="R7" s="94" t="s">
-        <v>109</v>
-      </c>
-      <c r="S7" s="86" t="s">
-        <v>104</v>
-      </c>
-      <c r="T7" s="85" t="s">
-        <v>97</v>
+      <c r="R7" s="92" t="s">
+        <v>103</v>
+      </c>
+      <c r="S7" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="T7" s="83" t="s">
+        <v>91</v>
       </c>
       <c r="U7" s="21"/>
     </row>
@@ -2315,14 +2319,14 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="57"/>
-      <c r="R8" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="S8" s="86" t="s">
-        <v>105</v>
-      </c>
-      <c r="T8" s="91" t="s">
-        <v>98</v>
+      <c r="R8" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="S8" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="T8" s="89" t="s">
+        <v>92</v>
       </c>
       <c r="U8" s="5"/>
     </row>
@@ -2352,14 +2356,14 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="57"/>
-      <c r="R9" s="92" t="s">
-        <v>111</v>
-      </c>
-      <c r="S9" s="93" t="s">
-        <v>106</v>
-      </c>
-      <c r="T9" s="95" t="s">
-        <v>99</v>
+      <c r="R9" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="S9" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="T9" s="93" t="s">
+        <v>93</v>
       </c>
       <c r="U9" s="21"/>
     </row>
@@ -2389,14 +2393,14 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="94" t="s">
-        <v>112</v>
-      </c>
-      <c r="S10" s="84" t="s">
-        <v>107</v>
-      </c>
-      <c r="T10" s="85" t="s">
-        <v>100</v>
+      <c r="R10" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="S10" s="82" t="s">
+        <v>101</v>
+      </c>
+      <c r="T10" s="83" t="s">
+        <v>94</v>
       </c>
       <c r="U10" s="21"/>
     </row>
@@ -2426,14 +2430,14 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="92" t="s">
-        <v>113</v>
-      </c>
-      <c r="S11" s="88" t="s">
-        <v>108</v>
-      </c>
-      <c r="T11" s="89" t="s">
-        <v>101</v>
+      <c r="R11" s="90" t="s">
+        <v>107</v>
+      </c>
+      <c r="S11" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="T11" s="87" t="s">
+        <v>95</v>
       </c>
       <c r="U11" s="21"/>
     </row>
@@ -2596,10 +2600,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="58"/>
+      <c r="F2" s="94"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -2675,12 +2679,12 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="82" t="s">
-        <v>116</v>
-      </c>
-      <c r="T5" s="83" t="s">
-        <v>123</v>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" s="81" t="s">
+        <v>117</v>
       </c>
       <c r="U5" s="21"/>
     </row>
@@ -2707,12 +2711,12 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="T6" s="85" t="s">
-        <v>124</v>
+      <c r="R6" s="79"/>
+      <c r="S6" s="86" t="s">
+        <v>111</v>
+      </c>
+      <c r="T6" s="83" t="s">
+        <v>118</v>
       </c>
       <c r="U6" s="21"/>
     </row>
@@ -2741,14 +2745,14 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="82" t="s">
-        <v>130</v>
-      </c>
-      <c r="S7" s="86" t="s">
-        <v>118</v>
-      </c>
-      <c r="T7" s="85" t="s">
-        <v>125</v>
+      <c r="R7" s="80" t="s">
+        <v>124</v>
+      </c>
+      <c r="S7" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="T7" s="83" t="s">
+        <v>119</v>
       </c>
       <c r="U7" s="21"/>
     </row>
@@ -2777,14 +2781,14 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="S8" s="90" t="s">
-        <v>119</v>
-      </c>
-      <c r="T8" s="91" t="s">
-        <v>126</v>
+      <c r="R8" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="S8" s="88" t="s">
+        <v>113</v>
+      </c>
+      <c r="T8" s="89" t="s">
+        <v>120</v>
       </c>
       <c r="U8" s="5"/>
     </row>
@@ -2813,14 +2817,14 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="92" t="s">
-        <v>132</v>
-      </c>
-      <c r="S9" s="93" t="s">
-        <v>120</v>
-      </c>
-      <c r="T9" s="85" t="s">
-        <v>127</v>
+      <c r="R9" s="90" t="s">
+        <v>126</v>
+      </c>
+      <c r="S9" s="91" t="s">
+        <v>114</v>
+      </c>
+      <c r="T9" s="83" t="s">
+        <v>121</v>
       </c>
       <c r="U9" s="21"/>
     </row>
@@ -2847,12 +2851,12 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="83"/>
-      <c r="S10" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="T10" s="89" t="s">
-        <v>128</v>
+      <c r="R10" s="81"/>
+      <c r="S10" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="T10" s="87" t="s">
+        <v>122</v>
       </c>
       <c r="U10" s="21"/>
     </row>
@@ -2866,10 +2870,10 @@
       <c r="F11" s="1"/>
       <c r="G11" s="13"/>
       <c r="H11" s="27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J11" s="21"/>
       <c r="M11" s="1">
@@ -2879,12 +2883,12 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="88" t="s">
-        <v>122</v>
-      </c>
-      <c r="T11" s="89" t="s">
-        <v>129</v>
+      <c r="R11" s="83"/>
+      <c r="S11" s="86" t="s">
+        <v>116</v>
+      </c>
+      <c r="T11" s="87" t="s">
+        <v>123</v>
       </c>
       <c r="U11" s="21"/>
     </row>
@@ -3044,10 +3048,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="58"/>
+      <c r="F2" s="94"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -3123,12 +3127,12 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="T5" s="83" t="s">
-        <v>95</v>
+      <c r="R5" s="79"/>
+      <c r="S5" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="T5" s="81" t="s">
+        <v>89</v>
       </c>
       <c r="U5" s="1"/>
     </row>
@@ -3155,12 +3159,12 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="84" t="s">
-        <v>103</v>
-      </c>
-      <c r="T6" s="85" t="s">
-        <v>96</v>
+      <c r="R6" s="79"/>
+      <c r="S6" s="82" t="s">
+        <v>97</v>
+      </c>
+      <c r="T6" s="83" t="s">
+        <v>90</v>
       </c>
       <c r="U6" s="1"/>
     </row>
@@ -3189,14 +3193,14 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="82" t="s">
-        <v>109</v>
-      </c>
-      <c r="S7" s="86" t="s">
-        <v>104</v>
-      </c>
-      <c r="T7" s="85" t="s">
-        <v>97</v>
+      <c r="R7" s="80" t="s">
+        <v>103</v>
+      </c>
+      <c r="S7" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="T7" s="83" t="s">
+        <v>91</v>
       </c>
       <c r="U7" s="1"/>
     </row>
@@ -3225,14 +3229,14 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="S8" s="86" t="s">
-        <v>105</v>
-      </c>
-      <c r="T8" s="87" t="s">
-        <v>98</v>
+      <c r="R8" s="82" t="s">
+        <v>104</v>
+      </c>
+      <c r="S8" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="T8" s="85" t="s">
+        <v>92</v>
       </c>
       <c r="U8" s="2"/>
     </row>
@@ -3261,14 +3265,14 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="88" t="s">
-        <v>111</v>
-      </c>
-      <c r="S9" s="87" t="s">
-        <v>106</v>
-      </c>
-      <c r="T9" s="85" t="s">
-        <v>99</v>
+      <c r="R9" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="S9" s="85" t="s">
+        <v>100</v>
+      </c>
+      <c r="T9" s="83" t="s">
+        <v>93</v>
       </c>
       <c r="U9" s="1"/>
     </row>
@@ -3295,12 +3299,12 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="83"/>
-      <c r="S10" s="84" t="s">
-        <v>107</v>
-      </c>
-      <c r="T10" s="85" t="s">
-        <v>100</v>
+      <c r="R10" s="81"/>
+      <c r="S10" s="82" t="s">
+        <v>101</v>
+      </c>
+      <c r="T10" s="83" t="s">
+        <v>94</v>
       </c>
       <c r="U10" s="1"/>
     </row>
@@ -3327,12 +3331,12 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="88" t="s">
-        <v>108</v>
-      </c>
-      <c r="T11" s="89" t="s">
-        <v>101</v>
+      <c r="R11" s="83"/>
+      <c r="S11" s="86" t="s">
+        <v>102</v>
+      </c>
+      <c r="T11" s="87" t="s">
+        <v>95</v>
       </c>
       <c r="U11" s="1"/>
     </row>

</xml_diff>

<commit_message>
Migrate third floor to use new way of handling rooms with Invoke-OGDRoom.ps1
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="First floor" sheetId="1" r:id="rId1"/>
     <sheet name="Second floor" sheetId="2" r:id="rId2"/>
     <sheet name="Third floor" sheetId="3" r:id="rId3"/>
     <sheet name="Fourth floor" sheetId="4" r:id="rId4"/>
+    <sheet name="Fifth floor" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
   <si>
     <t>y/x</t>
   </si>
@@ -432,6 +432,12 @@
   </si>
   <si>
     <t>Coord.</t>
+  </si>
+  <si>
+    <t>Airco</t>
+  </si>
+  <si>
+    <t>4e verdieping (Z=4)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1020,6 +1026,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1342,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,7 +2143,7 @@
   <dimension ref="B1:U15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3469,4 +3496,414 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:U15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="10" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="G2" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="94"/>
+      <c r="I2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="1">
+        <v>12</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="6"/>
+      <c r="M4" s="1">
+        <v>11</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="6"/>
+      <c r="M5" s="1">
+        <v>10</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6"/>
+      <c r="M6" s="1">
+        <v>9</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="97" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="6"/>
+      <c r="M7" s="1">
+        <v>8</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="50"/>
+      <c r="T7" s="99" t="s">
+        <v>91</v>
+      </c>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="96" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="21"/>
+      <c r="M8" s="1">
+        <v>7</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="100" t="s">
+        <v>99</v>
+      </c>
+      <c r="T8" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="1">
+        <v>6</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="50"/>
+      <c r="T9" s="102" t="s">
+        <v>93</v>
+      </c>
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="6"/>
+      <c r="M10" s="1">
+        <v>5</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="6"/>
+      <c r="M11" s="1">
+        <v>4</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="6"/>
+      <c r="M12" s="1">
+        <v>3</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="M13" s="1">
+        <v>2</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+    </row>
+    <row r="14" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="31"/>
+      <c r="M14" s="1">
+        <v>1</v>
+      </c>
+      <c r="N14" s="27"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+    </row>
+    <row r="15" spans="2:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15" s="4">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>6</v>
+      </c>
+      <c r="I15" s="4">
+        <v>7</v>
+      </c>
+      <c r="J15" s="4">
+        <v>8</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>1</v>
+      </c>
+      <c r="O15" s="1">
+        <v>2</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>4</v>
+      </c>
+      <c r="R15" s="4">
+        <v>5</v>
+      </c>
+      <c r="S15" s="4">
+        <v>6</v>
+      </c>
+      <c r="T15" s="4">
+        <v>7</v>
+      </c>
+      <c r="U15" s="4">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add penetration possibility 'Het pand binnengelopen'
</commit_message>
<xml_diff>
--- a/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
+++ b/PowerSpel-PenTest/Private/Rooms/FloorPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="First floor" sheetId="1" r:id="rId1"/>
@@ -744,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -846,9 +846,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1021,31 +1018,37 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1370,7 +1373,7 @@
   <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,20 +1385,20 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="94" t="s">
+      <c r="Q1" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="53" t="s">
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="52" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="F2" s="94" t="s">
+      <c r="F2" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="94"/>
+      <c r="G2" s="100"/>
       <c r="H2">
         <v>53</v>
       </c>
@@ -1415,7 +1418,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="N3" s="50">
+      <c r="N3" s="49">
         <v>12</v>
       </c>
       <c r="O3" s="5"/>
@@ -1452,38 +1455,38 @@
       <c r="I4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="38" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
-      <c r="N4" s="50">
+      <c r="N4" s="49">
         <v>11</v>
       </c>
       <c r="O4" s="5"/>
       <c r="P4" s="6"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="66" t="str">
+      <c r="Q4" s="64"/>
+      <c r="R4" s="65" t="str">
         <f>CONCATENATE(R15,N4,)</f>
         <v>0411</v>
       </c>
-      <c r="S4" s="66" t="str">
+      <c r="S4" s="65" t="str">
         <f>CONCATENATE(S15,N4,)</f>
         <v>0511</v>
       </c>
-      <c r="T4" s="66" t="str">
+      <c r="T4" s="65" t="str">
         <f>CONCATENATE(T15,N4)</f>
         <v>0611</v>
       </c>
-      <c r="U4" s="66" t="str">
+      <c r="U4" s="65" t="str">
         <f>CONCATENATE(U15,N4)</f>
         <v>0711</v>
       </c>
-      <c r="V4" s="66" t="str">
+      <c r="V4" s="65" t="str">
         <f>CONCATENATE(V15,N4)</f>
         <v>0811</v>
       </c>
-      <c r="W4" s="65" t="str">
+      <c r="W4" s="64" t="str">
         <f>CONCATENATE(W15,N4)</f>
         <v>0911</v>
       </c>
@@ -1500,47 +1503,47 @@
       <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="38" t="s">
         <v>9</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
-      <c r="N5" s="50">
+      <c r="N5" s="49">
         <v>10</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="6"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="66" t="str">
+      <c r="Q5" s="66"/>
+      <c r="R5" s="65" t="str">
         <f>CONCATENATE(R15,N5,)</f>
         <v>0410</v>
       </c>
-      <c r="S5" s="68" t="str">
+      <c r="S5" s="67" t="str">
         <f>CONCATENATE(S15,N5,)</f>
         <v>0510</v>
       </c>
-      <c r="T5" s="69" t="str">
+      <c r="T5" s="68" t="str">
         <f>CONCATENATE(T15,N5)</f>
         <v>0610</v>
       </c>
-      <c r="U5" s="70" t="str">
+      <c r="U5" s="69" t="str">
         <f>CONCATENATE(U15,N5)</f>
         <v>0710</v>
       </c>
-      <c r="V5" s="54"/>
-      <c r="W5" s="65" t="str">
+      <c r="V5" s="53"/>
+      <c r="W5" s="64" t="str">
         <f>CONCATENATE(W15,N5)</f>
         <v>0910</v>
       </c>
@@ -1559,50 +1562,50 @@
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="F6" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="38" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
-      <c r="N6" s="50" t="s">
+      <c r="N6" s="49" t="s">
         <v>86</v>
       </c>
       <c r="O6" s="5"/>
       <c r="P6" s="13"/>
-      <c r="Q6" s="66" t="str">
+      <c r="Q6" s="65" t="str">
         <f>CONCATENATE(Q15,N6,)</f>
         <v>0309</v>
       </c>
-      <c r="R6" s="66" t="str">
+      <c r="R6" s="65" t="str">
         <f>CONCATENATE(R15,N6,)</f>
         <v>0409</v>
       </c>
-      <c r="S6" s="71" t="str">
+      <c r="S6" s="70" t="str">
         <f>CONCATENATE(S15,N6,)</f>
         <v>0509</v>
       </c>
-      <c r="T6" s="64" t="str">
+      <c r="T6" s="63" t="str">
         <f>CONCATENATE(T15,N6)</f>
         <v>0609</v>
       </c>
-      <c r="U6" s="72" t="str">
+      <c r="U6" s="71" t="str">
         <f>CONCATENATE(U15,N6)</f>
         <v>0709</v>
       </c>
-      <c r="V6" s="55"/>
-      <c r="W6" s="65" t="str">
+      <c r="V6" s="54"/>
+      <c r="W6" s="64" t="str">
         <f>CONCATENATE(W15,N6)</f>
         <v>0909</v>
       </c>
@@ -1627,44 +1630,44 @@
       <c r="G7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="56" t="s">
+      <c r="I7" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="38" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-      <c r="N7" s="50" t="s">
+      <c r="N7" s="49" t="s">
         <v>85</v>
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="13"/>
-      <c r="Q7" s="66" t="str">
+      <c r="Q7" s="65" t="str">
         <f>CONCATENATE(Q15,N7,)</f>
         <v>0308</v>
       </c>
-      <c r="R7" s="73" t="str">
+      <c r="R7" s="72" t="str">
         <f>CONCATENATE(R15,N7,)</f>
         <v>0408</v>
       </c>
-      <c r="S7" s="74" t="str">
+      <c r="S7" s="73" t="str">
         <f>CONCATENATE(S15,N7)</f>
         <v>0508</v>
       </c>
-      <c r="T7" s="60" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE(T15,N7)</f>
         <v>0608</v>
       </c>
-      <c r="U7" s="75" t="str">
+      <c r="U7" s="74" t="str">
         <f>CONCATENATE(U15,N7)</f>
         <v>0708</v>
       </c>
-      <c r="V7" s="56"/>
-      <c r="W7" s="65" t="str">
+      <c r="V7" s="55"/>
+      <c r="W7" s="64" t="str">
         <f>CONCATENATE(W15,N7)</f>
         <v>0908</v>
       </c>
@@ -1695,41 +1698,41 @@
       <c r="I8" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="40" t="s">
+      <c r="J8" s="39" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
-      <c r="N8" s="50" t="s">
+      <c r="N8" s="49" t="s">
         <v>84</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="13"/>
-      <c r="Q8" s="66" t="str">
+      <c r="Q8" s="65" t="str">
         <f>CONCATENATE(Q15,N8,)</f>
         <v>0307</v>
       </c>
-      <c r="R8" s="63" t="str">
+      <c r="R8" s="62" t="str">
         <f>CONCATENATE(R15,N8,)</f>
         <v>0407</v>
       </c>
-      <c r="S8" s="76" t="str">
+      <c r="S8" s="75" t="str">
         <f>CONCATENATE(S15,N8)</f>
         <v>0507</v>
       </c>
-      <c r="T8" s="76" t="str">
+      <c r="T8" s="75" t="str">
         <f>CONCATENATE(T15,N8)</f>
         <v>0607</v>
       </c>
-      <c r="U8" s="62" t="str">
+      <c r="U8" s="61" t="str">
         <f>CONCATENATE(U15,N8)</f>
         <v>0707</v>
       </c>
-      <c r="V8" s="60" t="str">
+      <c r="V8" s="59" t="str">
         <f>CONCATENATE(V15,N8)</f>
         <v>0807</v>
       </c>
-      <c r="W8" s="60" t="str">
+      <c r="W8" s="59" t="str">
         <f>CONCATENATE(W15,N8)</f>
         <v>0907</v>
       </c>
@@ -1754,44 +1757,44 @@
       <c r="G9" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="38" t="s">
         <v>9</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
-      <c r="N9" s="50" t="s">
+      <c r="N9" s="49" t="s">
         <v>83</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="13"/>
-      <c r="Q9" s="60" t="str">
+      <c r="Q9" s="59" t="str">
         <f>CONCATENATE(Q15,N9,)</f>
         <v>0306</v>
       </c>
-      <c r="R9" s="61" t="str">
+      <c r="R9" s="60" t="str">
         <f>CONCATENATE(R15,N9,)</f>
         <v>0406</v>
       </c>
-      <c r="S9" s="62" t="str">
+      <c r="S9" s="61" t="str">
         <f>CONCATENATE(S15,N9)</f>
         <v>0506</v>
       </c>
-      <c r="T9" s="58" t="str">
+      <c r="T9" s="57" t="str">
         <f>CONCATENATE(T15,N9)</f>
         <v>0606</v>
       </c>
-      <c r="U9" s="75" t="str">
+      <c r="U9" s="74" t="str">
         <f>CONCATENATE(U15,N9)</f>
         <v>0706</v>
       </c>
-      <c r="V9" s="54"/>
-      <c r="W9" s="65" t="str">
+      <c r="V9" s="53"/>
+      <c r="W9" s="64" t="str">
         <f>CONCATENATE(W15,N9)</f>
         <v>0906</v>
       </c>
@@ -1804,13 +1807,13 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="37" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="42" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="33" t="s">
@@ -1819,41 +1822,41 @@
       <c r="H10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="38" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
-      <c r="N10" s="50" t="s">
+      <c r="N10" s="49" t="s">
         <v>82</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="13"/>
-      <c r="Q10" s="62" t="str">
+      <c r="Q10" s="61" t="str">
         <f>CONCATENATE(Q15,N10,)</f>
         <v>0305</v>
       </c>
-      <c r="R10" s="66" t="str">
+      <c r="R10" s="65" t="str">
         <f>CONCATENATE(R15,N10,)</f>
         <v>0405</v>
       </c>
-      <c r="S10" s="77" t="str">
+      <c r="S10" s="76" t="str">
         <f>CONCATENATE(S15,N10)</f>
         <v>0505</v>
       </c>
-      <c r="T10" s="59" t="str">
+      <c r="T10" s="58" t="str">
         <f>CONCATENATE(T15,N10)</f>
         <v>0605</v>
       </c>
-      <c r="U10" s="65" t="str">
+      <c r="U10" s="64" t="str">
         <f>CONCATENATE(U15,N10)</f>
         <v>0705</v>
       </c>
-      <c r="V10" s="55"/>
-      <c r="W10" s="65" t="str">
+      <c r="V10" s="54"/>
+      <c r="W10" s="64" t="str">
         <f>CONCATENATE(W15,N10)</f>
         <v>0905</v>
       </c>
@@ -1879,38 +1882,38 @@
       <c r="H11" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
         <v>9</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="N11" s="50" t="s">
+      <c r="N11" s="49" t="s">
         <v>81</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="66" t="str">
+      <c r="Q11" s="64"/>
+      <c r="R11" s="65" t="str">
         <f>CONCATENATE(R15,N11,)</f>
         <v>0404</v>
       </c>
-      <c r="S11" s="78" t="str">
+      <c r="S11" s="77" t="str">
         <f>CONCATENATE(S15,N11)</f>
         <v>0504</v>
       </c>
-      <c r="T11" s="62" t="str">
+      <c r="T11" s="61" t="str">
         <f>CONCATENATE(T15,N11)</f>
         <v>0604</v>
       </c>
-      <c r="U11" s="67" t="str">
+      <c r="U11" s="66" t="str">
         <f>CONCATENATE(U15,N11)</f>
         <v>0704</v>
       </c>
-      <c r="V11" s="56"/>
-      <c r="W11" s="65" t="str">
+      <c r="V11" s="55"/>
+      <c r="W11" s="64" t="str">
         <f>CONCATENATE(W15,N11)</f>
         <v>0904</v>
       </c>
@@ -1924,53 +1927,53 @@
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="F12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="J12" s="40" t="s">
         <v>9</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
-      <c r="N12" s="50" t="s">
+      <c r="N12" s="49" t="s">
         <v>80</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="62" t="str">
+      <c r="Q12" s="64"/>
+      <c r="R12" s="61" t="str">
         <f>CONCATENATE(R15,N12,)</f>
         <v>0403</v>
       </c>
-      <c r="S12" s="62" t="str">
+      <c r="S12" s="61" t="str">
         <f>CONCATENATE(S15,N12)</f>
         <v>0503</v>
       </c>
-      <c r="T12" s="62" t="str">
+      <c r="T12" s="61" t="str">
         <f>CONCATENATE(T15,N12)</f>
         <v>0603</v>
       </c>
-      <c r="U12" s="62" t="str">
+      <c r="U12" s="61" t="str">
         <f>CONCATENATE(U15,N12)</f>
         <v>0703</v>
       </c>
-      <c r="V12" s="62" t="str">
+      <c r="V12" s="61" t="str">
         <f>CONCATENATE(V15,N12)</f>
         <v>0803</v>
       </c>
-      <c r="W12" s="67" t="str">
+      <c r="W12" s="66" t="str">
         <f>CONCATENATE(W15,N12)</f>
         <v>0903</v>
       </c>
@@ -1992,7 +1995,7 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="31"/>
-      <c r="N13" s="50" t="s">
+      <c r="N13" s="49" t="s">
         <v>79</v>
       </c>
       <c r="O13" s="5"/>
@@ -2022,7 +2025,7 @@
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
       <c r="L14" s="31"/>
-      <c r="N14" s="50" t="s">
+      <c r="N14" s="49" t="s">
         <v>78</v>
       </c>
       <c r="O14" s="27"/>
@@ -2074,34 +2077,34 @@
       <c r="N15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O15" s="50" t="s">
+      <c r="O15" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="P15" s="50" t="s">
+      <c r="P15" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="Q15" s="50" t="s">
+      <c r="Q15" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="R15" s="51" t="s">
+      <c r="R15" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="S15" s="52" t="s">
+      <c r="S15" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="T15" s="52" t="s">
+      <c r="T15" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="U15" s="52" t="s">
+      <c r="U15" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="V15" s="52" t="s">
+      <c r="V15" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="W15" s="51" t="s">
+      <c r="W15" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="X15" s="50">
+      <c r="X15" s="49">
         <v>10</v>
       </c>
       <c r="AF15" s="1"/>
@@ -2117,11 +2120,11 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="95" t="s">
+      <c r="B20" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="101"/>
       <c r="E20">
         <f>SUM(H2,'Second floor'!I2,'Third floor'!G2,'Fourth floor'!G2)</f>
         <v>106</v>
@@ -2142,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,10 +2162,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="G2" s="94" t="s">
+      <c r="G2" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="94"/>
+      <c r="H2" s="100"/>
       <c r="I2">
         <v>19</v>
       </c>
@@ -2241,11 +2244,11 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="80" t="s">
+      <c r="R5" s="78"/>
+      <c r="S5" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="T5" s="81" t="s">
+      <c r="T5" s="80" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="21"/>
@@ -2274,11 +2277,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="79"/>
-      <c r="S6" s="86" t="s">
+      <c r="R6" s="78"/>
+      <c r="S6" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="T6" s="83" t="s">
+      <c r="T6" s="82" t="s">
         <v>90</v>
       </c>
       <c r="U6" s="21"/>
@@ -2290,7 +2293,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="57"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="16" t="s">
         <v>49</v>
       </c>
@@ -2308,14 +2311,14 @@
       <c r="N7" s="5"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="92" t="s">
+      <c r="Q7" s="56"/>
+      <c r="R7" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="S7" s="84" t="s">
+      <c r="S7" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="83" t="s">
+      <c r="T7" s="82" t="s">
         <v>91</v>
       </c>
       <c r="U7" s="21"/>
@@ -2327,7 +2330,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="57"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
@@ -2345,14 +2348,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="57"/>
-      <c r="R8" s="82" t="s">
+      <c r="Q8" s="56"/>
+      <c r="R8" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="S8" s="84" t="s">
+      <c r="S8" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="89" t="s">
+      <c r="T8" s="88" t="s">
         <v>92</v>
       </c>
       <c r="U8" s="5"/>
@@ -2364,8 +2367,8 @@
       <c r="C9" s="5"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="26" t="s">
+      <c r="F9" s="56"/>
+      <c r="G9" s="103" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="32" t="s">
@@ -2382,14 +2385,14 @@
       <c r="N9" s="5"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="90" t="s">
+      <c r="Q9" s="56"/>
+      <c r="R9" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="S9" s="91" t="s">
+      <c r="S9" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="T9" s="93" t="s">
+      <c r="T9" s="92" t="s">
         <v>93</v>
       </c>
       <c r="U9" s="21"/>
@@ -2402,7 +2405,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="102" t="s">
         <v>52</v>
       </c>
       <c r="H10" s="5" t="s">
@@ -2420,13 +2423,13 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="92" t="s">
+      <c r="R10" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="S10" s="82" t="s">
+      <c r="S10" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="83" t="s">
+      <c r="T10" s="82" t="s">
         <v>94</v>
       </c>
       <c r="U10" s="21"/>
@@ -2439,7 +2442,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="35" t="s">
         <v>53</v>
       </c>
       <c r="H11" s="27" t="s">
@@ -2457,13 +2460,13 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="90" t="s">
+      <c r="R11" s="89" t="s">
         <v>107</v>
       </c>
-      <c r="S11" s="86" t="s">
+      <c r="S11" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="T11" s="87" t="s">
+      <c r="T11" s="86" t="s">
         <v>95</v>
       </c>
       <c r="U11" s="21"/>
@@ -2627,10 +2630,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E2" s="94" t="s">
+      <c r="E2" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="94"/>
+      <c r="F2" s="100"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -2706,11 +2709,11 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="80" t="s">
+      <c r="R5" s="78"/>
+      <c r="S5" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="T5" s="81" t="s">
+      <c r="T5" s="80" t="s">
         <v>117</v>
       </c>
       <c r="U5" s="21"/>
@@ -2738,11 +2741,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="79"/>
-      <c r="S6" s="86" t="s">
+      <c r="R6" s="78"/>
+      <c r="S6" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="T6" s="83" t="s">
+      <c r="T6" s="82" t="s">
         <v>118</v>
       </c>
       <c r="U6" s="21"/>
@@ -2772,13 +2775,13 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="80" t="s">
+      <c r="R7" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="S7" s="84" t="s">
+      <c r="S7" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="T7" s="83" t="s">
+      <c r="T7" s="82" t="s">
         <v>119</v>
       </c>
       <c r="U7" s="21"/>
@@ -2808,13 +2811,13 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="82" t="s">
+      <c r="R8" s="81" t="s">
         <v>125</v>
       </c>
-      <c r="S8" s="88" t="s">
+      <c r="S8" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="T8" s="89" t="s">
+      <c r="T8" s="88" t="s">
         <v>120</v>
       </c>
       <c r="U8" s="5"/>
@@ -2844,13 +2847,13 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="90" t="s">
+      <c r="R9" s="89" t="s">
         <v>126</v>
       </c>
-      <c r="S9" s="91" t="s">
+      <c r="S9" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="T9" s="83" t="s">
+      <c r="T9" s="82" t="s">
         <v>121</v>
       </c>
       <c r="U9" s="21"/>
@@ -2878,11 +2881,11 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="82" t="s">
+      <c r="R10" s="80"/>
+      <c r="S10" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="T10" s="87" t="s">
+      <c r="T10" s="86" t="s">
         <v>122</v>
       </c>
       <c r="U10" s="21"/>
@@ -2910,11 +2913,11 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="83"/>
-      <c r="S11" s="86" t="s">
+      <c r="R11" s="82"/>
+      <c r="S11" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="T11" s="87" t="s">
+      <c r="T11" s="86" t="s">
         <v>123</v>
       </c>
       <c r="U11" s="21"/>
@@ -3075,10 +3078,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E2" s="94" t="s">
+      <c r="E2" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="94"/>
+      <c r="F2" s="100"/>
       <c r="G2">
         <v>17</v>
       </c>
@@ -3154,11 +3157,11 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="80" t="s">
+      <c r="R5" s="78"/>
+      <c r="S5" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="T5" s="81" t="s">
+      <c r="T5" s="80" t="s">
         <v>89</v>
       </c>
       <c r="U5" s="1"/>
@@ -3186,11 +3189,11 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="79"/>
-      <c r="S6" s="82" t="s">
+      <c r="R6" s="78"/>
+      <c r="S6" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="T6" s="83" t="s">
+      <c r="T6" s="82" t="s">
         <v>90</v>
       </c>
       <c r="U6" s="1"/>
@@ -3220,13 +3223,13 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="80" t="s">
+      <c r="R7" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="S7" s="84" t="s">
+      <c r="S7" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="83" t="s">
+      <c r="T7" s="82" t="s">
         <v>91</v>
       </c>
       <c r="U7" s="1"/>
@@ -3256,13 +3259,13 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="82" t="s">
+      <c r="R8" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="S8" s="84" t="s">
+      <c r="S8" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="85" t="s">
+      <c r="T8" s="84" t="s">
         <v>92</v>
       </c>
       <c r="U8" s="2"/>
@@ -3292,13 +3295,13 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="86" t="s">
+      <c r="R9" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="S9" s="85" t="s">
+      <c r="S9" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="T9" s="83" t="s">
+      <c r="T9" s="82" t="s">
         <v>93</v>
       </c>
       <c r="U9" s="1"/>
@@ -3326,11 +3329,11 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="81"/>
-      <c r="S10" s="82" t="s">
+      <c r="R10" s="80"/>
+      <c r="S10" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="T10" s="83" t="s">
+      <c r="T10" s="82" t="s">
         <v>94</v>
       </c>
       <c r="U10" s="1"/>
@@ -3358,11 +3361,11 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="83"/>
-      <c r="S11" s="86" t="s">
+      <c r="R11" s="82"/>
+      <c r="S11" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="T11" s="87" t="s">
+      <c r="T11" s="86" t="s">
         <v>95</v>
       </c>
       <c r="U11" s="1"/>
@@ -3502,7 +3505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -3519,10 +3522,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="G2" s="94" t="s">
+      <c r="G2" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="94"/>
+      <c r="H2" s="100"/>
       <c r="I2">
         <v>4</v>
       </c>
@@ -3637,7 +3640,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="97" t="s">
+      <c r="I7" s="94" t="s">
         <v>9</v>
       </c>
       <c r="J7" s="1"/>
@@ -3650,8 +3653,8 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="99" t="s">
+      <c r="S7" s="49"/>
+      <c r="T7" s="96" t="s">
         <v>91</v>
       </c>
       <c r="U7" s="1"/>
@@ -3665,10 +3668,10 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="96" t="s">
+      <c r="H8" s="93" t="s">
         <v>135</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="56" t="s">
         <v>56</v>
       </c>
       <c r="J8" s="1"/>
@@ -3681,10 +3684,10 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="100" t="s">
+      <c r="S8" s="97" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="101" t="s">
+      <c r="T8" s="98" t="s">
         <v>92</v>
       </c>
       <c r="U8" s="1"/>
@@ -3699,7 +3702,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="98" t="s">
+      <c r="I9" s="95" t="s">
         <v>9</v>
       </c>
       <c r="J9" s="1"/>
@@ -3712,8 +3715,8 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="50"/>
-      <c r="T9" s="102" t="s">
+      <c r="S9" s="49"/>
+      <c r="T9" s="99" t="s">
         <v>93</v>
       </c>
       <c r="U9" s="1"/>

</xml_diff>